<commit_message>
survey, monthly, weekly, and weeklyYear classes udpated
</commit_message>
<xml_diff>
--- a/Year3_Project/Documents/Evaluations/Weekly Comparison.xlsx
+++ b/Year3_Project/Documents/Evaluations/Weekly Comparison.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="2720" yWindow="-80" windowWidth="21600" windowHeight="15320" tabRatio="500"/>
+    <workbookView xWindow="-20" yWindow="-20" windowWidth="21600" windowHeight="15320" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -329,187 +329,187 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="61"/>
                 <c:pt idx="0">
-                  <c:v>0.322207701606061</c:v>
+                  <c:v>0.170891063275283</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.246610098429972</c:v>
+                  <c:v>0.176734624494346</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.244371208698962</c:v>
+                  <c:v>0.189655529393182</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.24307133658799</c:v>
+                  <c:v>0.190269088468723</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.241970344239566</c:v>
+                  <c:v>0.18579585650666</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.241020385863951</c:v>
+                  <c:v>0.182765517322699</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.240161182912681</c:v>
+                  <c:v>0.179319716808685</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.239359625924868</c:v>
+                  <c:v>0.174464241845423</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.238598434441911</c:v>
+                  <c:v>0.170802133462548</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.237868198716413</c:v>
+                  <c:v>0.168570445993694</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.237163442524114</c:v>
+                  <c:v>0.167612878029524</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.236480717977958</c:v>
+                  <c:v>0.167095237103902</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.235817665539432</c:v>
+                  <c:v>0.1668394964107</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.235172542750797</c:v>
+                  <c:v>0.166666772436607</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.234543987215304</c:v>
+                  <c:v>0.166514514398946</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.233930898980787</c:v>
+                  <c:v>0.16636592861863</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.233332384062157</c:v>
+                  <c:v>0.166200331154002</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.232747728404397</c:v>
+                  <c:v>0.165975014412715</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.232176385224999</c:v>
+                  <c:v>0.165597329195588</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.231617965479528</c:v>
+                  <c:v>0.164875003659872</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0.231072224738051</c:v>
+                  <c:v>0.163513597041372</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>0.230539041984793</c:v>
+                  <c:v>0.161432625392691</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>0.230018387869719</c:v>
+                  <c:v>0.159283552632882</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>0.229510282309644</c:v>
+                  <c:v>0.157832845861242</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>0.229014744108284</c:v>
+                  <c:v>0.157088083235906</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>0.22853173798573</c:v>
+                  <c:v>0.156736964206873</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>0.228061126274667</c:v>
+                  <c:v>0.156564748772609</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>0.227602632768211</c:v>
+                  <c:v>0.15647099879605</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>0.227155824481439</c:v>
+                  <c:v>0.156413260150052</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>0.226720113841414</c:v>
+                  <c:v>0.156373615807565</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>0.226294780070066</c:v>
+                  <c:v>0.156344144680854</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>0.225879005408118</c:v>
+                  <c:v>0.156321062487683</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>0.225471920097044</c:v>
+                  <c:v>0.156302374631209</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>0.225072649826302</c:v>
+                  <c:v>0.156286913269957</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>0.224680360301337</c:v>
+                  <c:v>0.156273925610435</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>0.224294295123161</c:v>
+                  <c:v>0.156262887800976</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>0.223913804779726</c:v>
+                  <c:v>0.156253414755249</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>0.223538365908637</c:v>
+                  <c:v>0.156245212770111</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>0.22316759097231</c:v>
+                  <c:v>0.156238052379551</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>0.222801229105603</c:v>
+                  <c:v>0.156231751456642</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>0.222439159245096</c:v>
+                  <c:v>0.156226163915857</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>0.22208137684463</c:v>
+                  <c:v>0.156221171723704</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>0.221727975619123</c:v>
+                  <c:v>0.1562166790103</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>0.221379125885151</c:v>
+                  <c:v>0.156212607599638</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>0.221035051171337</c:v>
+                  <c:v>0.156208893545365</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>0.220696004801821</c:v>
+                  <c:v>0.156205484405677</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>0.220362248053046</c:v>
+                  <c:v>0.15620233707632</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>0.220034031218575</c:v>
+                  <c:v>0.156199416053496</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>0.219711578509827</c:v>
+                  <c:v>0.156196692032856</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>0.219395077237724</c:v>
+                  <c:v>0.156194140774317</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>0.219084671247326</c:v>
+                  <c:v>0.156191742178992</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>0.218780458189557</c:v>
+                  <c:v>0.15618947953661</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>0.218482489957096</c:v>
+                  <c:v>0.156187338910753</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>0.21819077549411</c:v>
+                  <c:v>0.156185308635994</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>0.217905285192209</c:v>
+                  <c:v>0.156183378906252</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>0.217625956172457</c:v>
+                  <c:v>0.156181541437664</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>0.217352697886569</c:v>
+                  <c:v>0.156179789192492</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>0.217085397617728</c:v>
+                  <c:v>0.15617811615307</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>0.216823925599585</c:v>
+                  <c:v>0.156176517136831</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>0.216568139588484</c:v>
+                  <c:v>0.156174987645053</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>0.216317888814062</c:v>
+                  <c:v>0.156173523739307</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -733,187 +733,187 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="61"/>
                 <c:pt idx="0">
-                  <c:v>0.10381780297426</c:v>
+                  <c:v>0.0292037555073571</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.0608165406476406</c:v>
+                  <c:v>0.0312351274951576</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.0597172876409919</c:v>
+                  <c:v>0.0359692198294083</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.0590836746706723</c:v>
+                  <c:v>0.0362023260267188</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.0585496474914142</c:v>
+                  <c:v>0.0345201002950436</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.058090826402008</c:v>
+                  <c:v>0.033403234322234</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.0576773937780183</c:v>
+                  <c:v>0.0321555608363472</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.0572930305228931</c:v>
+                  <c:v>0.0304377716826984</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.0569292129181311</c:v>
+                  <c:v>0.0291733687953581</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.0565812799605912</c:v>
+                  <c:v>0.0284159952625131</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.0562464984698887</c:v>
+                  <c:v>0.0280940768813403</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.0559231299753707</c:v>
+                  <c:v>0.0279208182628094</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.0556099713804675</c:v>
+                  <c:v>0.0278354175625761</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.0553061248638758</c:v>
+                  <c:v>0.0277778130344359</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.0550108819388529</c:v>
+                  <c:v>0.0277270835055169</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.0547236654979594</c:v>
+                  <c:v>0.0276776222051391</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.0544440014521301</c:v>
+                  <c:v>0.0276225500757001</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.0541715050774073</c:v>
+                  <c:v>0.027547705409301</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.0539058738561472</c:v>
+                  <c:v>0.0274224754367121</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.0536468819328761</c:v>
+                  <c:v>0.0271837668318429</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0.0533943730453924</c:v>
+                  <c:v>0.0267366964174081</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>0.0531482498792664</c:v>
+                  <c:v>0.0260604925411769</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>0.0529084587581846</c:v>
+                  <c:v>0.0253712501393523</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>0.0526749696858525</c:v>
+                  <c:v>0.0249112072326587</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>0.0524477530189828</c:v>
+                  <c:v>0.0246766658947311</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>0.0522267552667783</c:v>
+                  <c:v>0.0245664759487868</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>0.0520118773176696</c:v>
+                  <c:v>0.0245125205582302</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>0.0518029584430212</c:v>
+                  <c:v>0.0244831734642337</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>0.0515997685958427</c:v>
+                  <c:v>0.0244651079507679</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>0.0514020100202641</c:v>
+                  <c:v>0.0244527077207322</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>0.0512093274869597</c:v>
+                  <c:v>0.024443491575988</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>0.051021325084161</c:v>
+                  <c:v>0.0244362745772782</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>0.0508375867522478</c:v>
+                  <c:v>0.024430432315355</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>0.0506576976998334</c:v>
+                  <c:v>0.024425599259451</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>0.050481264305139</c:v>
+                  <c:v>0.0244215398256958</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>0.0503079308247957</c:v>
+                  <c:v>0.0244180901039004</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>0.0501373919709332</c:v>
+                  <c:v>0.024415129622676</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>0.0499694010331037</c:v>
+                  <c:v>0.0244125665135774</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>0.0498037736603845</c:v>
+                  <c:v>0.0244103290113555</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>0.0496403876909673</c:v>
+                  <c:v>0.02440836016321</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>0.0494791795656653</c:v>
+                  <c:v>0.0244066142918644</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>0.0493201379412069</c:v>
+                  <c:v>0.0244050544947272</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>0.0491632951721545</c:v>
+                  <c:v>0.0244036508010071</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>0.0490087173776737</c:v>
+                  <c:v>0.0244023787730785</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>0.0488564938463157</c:v>
+                  <c:v>0.0244012184226674</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>0.0487067265354854</c:v>
+                  <c:v>0.0244001533584122</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>0.0485595203669922</c:v>
+                  <c:v>0.0243991701081044</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>0.0484149748942971</c:v>
+                  <c:v>0.0243982575754532</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>0.0482731777312799</c:v>
+                  <c:v>0.024397406602007</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>0.0481341999161473</c:v>
+                  <c:v>0.0243966096122272</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>0.047998093175549</c:v>
+                  <c:v>0.0243958603249087</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>0.0478648888856325</c:v>
+                  <c:v>0.0243951535179173</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>0.0477345984178529</c:v>
+                  <c:v>0.0243944848360224</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>0.0476072145107212</c:v>
+                  <c:v>0.0243938506337209</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>0.0474827133146981</c:v>
+                  <c:v>0.024393247846574</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>0.0473610567999763</c:v>
+                  <c:v>0.0243926738858449</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>0.0472421952785704</c:v>
+                  <c:v>0.0243921265522113</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>0.0471260698588471</c:v>
+                  <c:v>0.0243916039651219</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>0.0470126147124146</c:v>
+                  <c:v>0.0243911045049909</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>0.0469017590848172</c:v>
+                  <c:v>0.0243906267659326</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>0.0467934290209729</c:v>
+                  <c:v>0.0243901695171521</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1137,187 +1137,187 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="61"/>
                 <c:pt idx="0">
-                  <c:v>0.27168019428478</c:v>
+                  <c:v>0.248586037714733</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.2247480596355</c:v>
+                  <c:v>0.187277052781453</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.221983970434628</c:v>
+                  <c:v>0.182877923234987</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.224169435641819</c:v>
+                  <c:v>0.180541544926993</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.229450188781374</c:v>
+                  <c:v>0.178992220025623</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.233198878993336</c:v>
+                  <c:v>0.177875833951677</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.234937003562313</c:v>
+                  <c:v>0.17703874597737</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.235550044802046</c:v>
+                  <c:v>0.176395952295937</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.235610629423664</c:v>
+                  <c:v>0.175893689392955</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.235389028744789</c:v>
+                  <c:v>0.175495476486781</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.234645974187537</c:v>
+                  <c:v>0.175175651373729</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.233471187720673</c:v>
+                  <c:v>0.174915795932004</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.232288453903818</c:v>
+                  <c:v>0.174702504093542</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.231141803118564</c:v>
+                  <c:v>0.174525895000133</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.230035175627134</c:v>
+                  <c:v>0.174378593976684</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.228970645773965</c:v>
+                  <c:v>0.174255025486758</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.227949639244127</c:v>
+                  <c:v>0.174150918941337</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.226973017920588</c:v>
+                  <c:v>0.17406296085077</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.226041141652906</c:v>
+                  <c:v>0.173988547995724</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.225153933428061</c:v>
+                  <c:v>0.173925610651012</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0.224310945291502</c:v>
+                  <c:v>0.173872484693703</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>0.223511422268519</c:v>
+                  <c:v>0.17382781809272</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>0.222754362244852</c:v>
+                  <c:v>0.173790501799109</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>0.222038570434158</c:v>
+                  <c:v>0.173759618123402</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>0.221362707638684</c:v>
+                  <c:v>0.173734401772807</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>0.220725331987208</c:v>
+                  <c:v>0.173714210147448</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>0.220124934210754</c:v>
+                  <c:v>0.173698500477004</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>0.21955996679778</c:v>
+                  <c:v>0.173686812060817</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>0.219028867565015</c:v>
+                  <c:v>0.173678752352016</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>0.218530078298503</c:v>
+                  <c:v>0.173673985963677</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>0.218062059172906</c:v>
+                  <c:v>0.173672225916043</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>0.217623299657416</c:v>
+                  <c:v>0.173673226617454</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>0.217212326575949</c:v>
+                  <c:v>0.173676778198121</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>0.216827709919856</c:v>
+                  <c:v>0.17368270190885</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>0.216468066924491</c:v>
+                  <c:v>0.173690846365928</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>0.21613206482725</c:v>
+                  <c:v>0.173701084475269</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>0.215818422632041</c:v>
+                  <c:v>0.173713310908354</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>0.21552591211981</c:v>
+                  <c:v>0.173727440032865</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>0.21525335826965</c:v>
+                  <c:v>0.173743404224598</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>0.214999639190987</c:v>
+                  <c:v>0.173761152506178</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>0.214763685612171</c:v>
+                  <c:v>0.173780649473433</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>0.214544479918095</c:v>
+                  <c:v>0.173801874483252</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>0.214341054666355</c:v>
+                  <c:v>0.173824821087962</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>0.214152490409503</c:v>
+                  <c:v>0.173849496711556</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>0.21397791245086</c:v>
+                  <c:v>0.173875922572961</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>0.213816485740345</c:v>
+                  <c:v>0.173904133871557</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>0.213667406227566</c:v>
+                  <c:v>0.173934180260912</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>0.213529885146117</c:v>
+                  <c:v>0.173966126648869</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>0.213403118943936</c:v>
+                  <c:v>0.174000054376285</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>0.213286229888627</c:v>
+                  <c:v>0.174036062844057</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>0.213178146019807</c:v>
+                  <c:v>0.174074271679443</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>0.213077348520423</c:v>
+                  <c:v>0.174114823559784</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>0.212981221401285</c:v>
+                  <c:v>0.174157887846317</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>0.212882260196977</c:v>
+                  <c:v>0.174203665225425</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>0.212694425645286</c:v>
+                  <c:v>0.174252393612335</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>0.213287026197412</c:v>
+                  <c:v>0.174304355647055</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>0.213579440333556</c:v>
+                  <c:v>0.17435988820855</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>0.215270297171071</c:v>
+                  <c:v>0.174419394495838</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>0.217503768202045</c:v>
+                  <c:v>0.174483359377567</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>0.223132794684201</c:v>
+                  <c:v>0.174552368894824</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>0.234987398645275</c:v>
+                  <c:v>0.174627135004826</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1541,187 +1541,187 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="61"/>
                 <c:pt idx="0">
-                  <c:v>0.0738101279666162</c:v>
+                  <c:v>0.0617950181467108</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.0505116903099225</c:v>
+                  <c:v>0.0350726944985074</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.0492768831299218</c:v>
+                  <c:v>0.033444334806742</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.0502519358759719</c:v>
+                  <c:v>0.0325952494446254</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.0526473891318082</c:v>
+                  <c:v>0.0320382148297012</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.0543817171637488</c:v>
+                  <c:v>0.0316398123040048</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.0551953956428385</c:v>
+                  <c:v>0.0313427175772398</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.0554838236062462</c:v>
+                  <c:v>0.0311155319863906</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.0555123686974155</c:v>
+                  <c:v>0.0309385899682655</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.0554079948534154</c:v>
+                  <c:v>0.0307986622673226</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.0550587332024185</c:v>
+                  <c:v>0.0306865088342104</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.0545087954957021</c:v>
+                  <c:v>0.0305955356665266</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.0539579258170265</c:v>
+                  <c:v>0.0305209649365542</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.053426533148901</c:v>
+                  <c:v>0.0304592880255975</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.0529161820258066</c:v>
+                  <c:v>0.0304078940372854</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.0524275566261468</c:v>
+                  <c:v>0.0303648139073907</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.051961038031528</c:v>
+                  <c:v>0.0303285425681121</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.0515167508639795</c:v>
+                  <c:v>0.0302979143401367</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.0510945977197495</c:v>
+                  <c:v>0.0302720148336606</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.0506942937381277</c:v>
+                  <c:v>0.0302501180403276</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0.0503154001775674</c:v>
+                  <c:v>0.0302316409335622</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>0.0499573558844962</c:v>
+                  <c:v>0.030216110342876</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>0.049619505899111</c:v>
+                  <c:v>0.0302031385155863</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>0.0493011267604448</c:v>
+                  <c:v>0.0301924048903905</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>0.0490014483331298</c:v>
+                  <c:v>0.0301836423593551</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>0.0487196721808635</c:v>
+                  <c:v>0.0301766268071519</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>0.0484549866612887</c:v>
+                  <c:v>0.0301711690679597</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>0.0482065790202422</c:v>
+                  <c:v>0.0301671086838499</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>0.0479736448268128</c:v>
+                  <c:v>0.0301643090185532</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>0.0477553951211502</c:v>
+                  <c:v>0.0301626534005118</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>0.0475510616507283</c:v>
+                  <c:v>0.0301620420546331</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>0.0473599005537816</c:v>
+                  <c:v>0.0301623896437177</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>0.0471811948165369</c:v>
+                  <c:v>0.0301636232852793</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>0.0470142557890895</c:v>
+                  <c:v>0.0301656809423586</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>0.0468584239980262</c:v>
+                  <c:v>0.0301685101113126</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>0.0467130694464909</c:v>
+                  <c:v>0.0301720667478846</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>0.0465775915473826</c:v>
+                  <c:v>0.0301763143867427</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>0.0464514187950764</c:v>
+                  <c:v>0.0301812234203729</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>0.0463340082463627</c:v>
+                  <c:v>0.0301867705115523</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>0.0462248448522547</c:v>
+                  <c:v>0.0301929381202753</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>0.0461234406577236</c:v>
+                  <c:v>0.0301997141314082</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>0.0460293338633261</c:v>
+                  <c:v>0.0302070915738921</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>0.0459420877154855</c:v>
+                  <c:v>0.030215068426262</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>0.0458612891485925</c:v>
+                  <c:v>0.0302236475068614</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>0.045786547016828</c:v>
+                  <c:v>0.0302328364505986</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>0.0457174895743511</c:v>
+                  <c:v>0.0302426477776166</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>0.0456537604840157</c:v>
+                  <c:v>0.0302530990630356</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>0.045595011850514</c:v>
+                  <c:v>0.0302642132212103</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>0.0455408911749997</c:v>
+                  <c:v>0.0302760189229501</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>0.0454910158601045</c:v>
+                  <c:v>0.0302885511702606</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>0.0454449219404422</c:v>
+                  <c:v>0.0303018520607287</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>0.0454019564524938</c:v>
+                  <c:v>0.0303159717832547</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>0.0453610006695832</c:v>
+                  <c:v>0.0303309698990904</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>0.0453188567065735</c:v>
+                  <c:v>0.0303469169779722</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>0.0452389187005784</c:v>
+                  <c:v>0.0303638966796284</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>0.0454913555441357</c:v>
+                  <c:v>0.0303820083975352</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>0.0456161773331953</c:v>
+                  <c:v>0.0304013706160983</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>0.0463413008441215</c:v>
+                  <c:v>0.030422125176295</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>0.0473078891820889</c:v>
+                  <c:v>0.0304444426996812</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>0.0497882440635821</c:v>
+                  <c:v>0.0304685294867947</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>0.0552190775220737</c:v>
+                  <c:v>0.0304946362799937</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1945,187 +1945,187 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="61"/>
                 <c:pt idx="0">
-                  <c:v>0.279291229</c:v>
+                  <c:v>0.169241275988439</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.224252678</c:v>
+                  <c:v>0.156973001515738</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.209824084</c:v>
+                  <c:v>0.155885720566241</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.194149904</c:v>
+                  <c:v>0.156287576358033</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.188214208</c:v>
+                  <c:v>0.156539655488187</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.185115165</c:v>
+                  <c:v>0.156746298532659</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.183161262</c:v>
+                  <c:v>0.156946764427646</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.181809368</c:v>
+                  <c:v>0.157113986953844</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.180824552</c:v>
+                  <c:v>0.157234787280885</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.180084685</c:v>
+                  <c:v>0.157290948761065</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.179518256</c:v>
+                  <c:v>0.157237667018754</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.179079816</c:v>
+                  <c:v>0.157097477721355</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.178738712</c:v>
+                  <c:v>0.156950108101871</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.178473321</c:v>
+                  <c:v>0.156775342793769</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.178267847</c:v>
+                  <c:v>0.156479924462197</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.178110422</c:v>
+                  <c:v>0.156100854897301</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.177991923</c:v>
+                  <c:v>0.155728108838255</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.177905205</c:v>
+                  <c:v>0.155255506279528</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.177844577</c:v>
+                  <c:v>0.155766786902874</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.17780545</c:v>
+                  <c:v>0.157678785842452</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0.17778408</c:v>
+                  <c:v>0.15909211723042</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>0.177777379</c:v>
+                  <c:v>0.160431748627047</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>0.177782781</c:v>
+                  <c:v>0.161247059341444</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>0.17779814</c:v>
+                  <c:v>0.161192459601665</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>0.177821643</c:v>
+                  <c:v>0.159445048188595</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>0.177851759</c:v>
+                  <c:v>0.15803822863541</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>0.177887181</c:v>
+                  <c:v>0.157556503666126</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>0.177926793</c:v>
+                  <c:v>0.157193905253803</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>0.177969636</c:v>
+                  <c:v>0.156635723940393</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>0.178014885</c:v>
+                  <c:v>0.155984654824021</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>0.178061826</c:v>
+                  <c:v>0.155433243496393</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>0.178109839</c:v>
+                  <c:v>0.155035155721611</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>0.178158384</c:v>
+                  <c:v>0.154751782754102</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>0.17820699</c:v>
+                  <c:v>0.154542031586776</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>0.178255241</c:v>
+                  <c:v>0.154383330815537</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>0.178302768</c:v>
+                  <c:v>0.154264300036061</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>0.178349245</c:v>
+                  <c:v>0.154178545084271</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>0.178394375</c:v>
+                  <c:v>0.154125234678153</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>0.178437889</c:v>
+                  <c:v>0.154116126510043</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>0.17847954</c:v>
+                  <c:v>0.154168632120786</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>0.178519095</c:v>
+                  <c:v>0.154271742278836</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>0.17855633</c:v>
+                  <c:v>0.15439510051163</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>0.178591031</c:v>
+                  <c:v>0.154513454377253</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>0.178622981</c:v>
+                  <c:v>0.154613697166789</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>0.178651964</c:v>
+                  <c:v>0.154692036875237</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>0.178677757</c:v>
+                  <c:v>0.154749191540852</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>0.178700123</c:v>
+                  <c:v>0.15478727228059</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>0.178718814</c:v>
+                  <c:v>0.154808503033178</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>0.178733561</c:v>
+                  <c:v>0.154814868522846</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>0.17874407</c:v>
+                  <c:v>0.154808056572575</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>0.17875002</c:v>
+                  <c:v>0.154789468597659</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>0.178751059</c:v>
+                  <c:v>0.154760290373655</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>0.178746795</c:v>
+                  <c:v>0.154721691492993</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>0.178736793</c:v>
+                  <c:v>0.154675205091879</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>0.178720572</c:v>
+                  <c:v>0.154623200845203</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>0.178697596</c:v>
+                  <c:v>0.154569087821357</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>0.178667272</c:v>
+                  <c:v>0.15451675732677</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>0.178628939</c:v>
+                  <c:v>0.154469494159595</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>0.178581872</c:v>
+                  <c:v>0.154429839657681</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>0.17852527</c:v>
+                  <c:v>0.154401282859224</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>0.178458255</c:v>
+                  <c:v>0.154390133809026</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2349,187 +2349,187 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="61"/>
                 <c:pt idx="0">
-                  <c:v>0.07800359</c:v>
+                  <c:v>0.0286426094981949</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.050289264</c:v>
+                  <c:v>0.0246405232048601</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.044026146</c:v>
+                  <c:v>0.0243003578764564</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.037694185</c:v>
+                  <c:v>0.0244258065238682</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.035424588</c:v>
+                  <c:v>0.0245046637403604</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.034267624</c:v>
+                  <c:v>0.0245694021036896</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.033548048</c:v>
+                  <c:v>0.024632286864307</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.033054646</c:v>
+                  <c:v>0.0246848048965329</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.032697519</c:v>
+                  <c:v>0.0247227783312651</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.032430494</c:v>
+                  <c:v>0.0247404425621559</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.032226804</c:v>
+                  <c:v>0.0247236839295006</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.032069581</c:v>
+                  <c:v>0.0246796175064117</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.031947527</c:v>
+                  <c:v>0.0246333364331891</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.031852726</c:v>
+                  <c:v>0.024578508108104</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.031779425</c:v>
+                  <c:v>0.0244859667596949</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.031723322</c:v>
+                  <c:v>0.0243674768996683</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.031681125</c:v>
+                  <c:v>0.0242512438823396</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.031650262</c:v>
+                  <c:v>0.0241042722301126</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.031628693</c:v>
+                  <c:v>0.0242632919020453</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.031614778</c:v>
+                  <c:v>0.02486259950475</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0.031607179</c:v>
+                  <c:v>0.0253103017648577</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>0.031604796</c:v>
+                  <c:v>0.025738345967532</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>0.031606717</c:v>
+                  <c:v>0.0260006141462633</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>0.031612178</c:v>
+                  <c:v>0.0259830090324346</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>0.031620537</c:v>
+                  <c:v>0.0254227233918636</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>0.031631248</c:v>
+                  <c:v>0.0249760817102182</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>0.031643849</c:v>
+                  <c:v>0.024824051847494</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>0.031657944</c:v>
+                  <c:v>0.0247099238489416</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>0.031673191</c:v>
+                  <c:v>0.0245347500143312</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>0.031689299</c:v>
+                  <c:v>0.024331212540569</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>0.031706014</c:v>
+                  <c:v>0.0241594931838091</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>0.031723115</c:v>
+                  <c:v>0.0240358995096242</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>0.03174041</c:v>
+                  <c:v>0.023948114265573</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>0.031757731</c:v>
+                  <c:v>0.0238832395269682</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>0.031774931</c:v>
+                  <c:v>0.0238342128336998</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>0.031791877</c:v>
+                  <c:v>0.0237974742656159</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>0.031808453</c:v>
+                  <c:v>0.0237710237643026</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>0.031824553</c:v>
+                  <c:v>0.0237545879645959</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>0.03184008</c:v>
+                  <c:v>0.0237517804504598</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>0.031854946</c:v>
+                  <c:v>0.0237679671299942</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>0.031869067</c:v>
+                  <c:v>0.0237997704657478</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>0.031882363</c:v>
+                  <c:v>0.0238378470619963</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>0.031894756</c:v>
+                  <c:v>0.0238744075835916</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>0.031906169</c:v>
+                  <c:v>0.0239053953515836</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>0.031916524</c:v>
+                  <c:v>0.0239296262726098</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>0.031925741</c:v>
+                  <c:v>0.0239473122825475</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>0.031933734</c:v>
+                  <c:v>0.0239590996600656</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>0.031940415</c:v>
+                  <c:v>0.0239656726113736</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>0.031945686</c:v>
+                  <c:v>0.0239676435157462</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>0.031949442</c:v>
+                  <c:v>0.0239655343797777</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>0.03195157</c:v>
+                  <c:v>0.0239597795887457</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>0.031951941</c:v>
+                  <c:v>0.0239507474765382</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>0.031950417</c:v>
+                  <c:v>0.0239388018184529</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>0.031946841</c:v>
+                  <c:v>0.023924419070215</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>0.031941043</c:v>
+                  <c:v>0.0239083342396161</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>0.031932831</c:v>
+                  <c:v>0.0238916029099264</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>0.031921994</c:v>
+                  <c:v>0.02387542829478</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>0.031908298</c:v>
+                  <c:v>0.0238608246259211</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>0.031891485</c:v>
+                  <c:v>0.0238485753766971</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>0.031871272</c:v>
+                  <c:v>0.0238397561485741</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>0.031847349</c:v>
+                  <c:v>0.0238363134175692</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2753,187 +2753,187 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="61"/>
                 <c:pt idx="0">
-                  <c:v>0.253971228718373</c:v>
+                  <c:v>0.569168139449575</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.243844790235392</c:v>
+                  <c:v>0.376685604948931</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.238677287607731</c:v>
+                  <c:v>0.371887779934286</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.23602016527823</c:v>
+                  <c:v>0.369579409428629</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.233808954489202</c:v>
+                  <c:v>0.368116874116947</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.232387906892622</c:v>
+                  <c:v>0.367077160839816</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.231228308604726</c:v>
+                  <c:v>0.366286998575045</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.230359709149584</c:v>
+                  <c:v>0.365659500279336</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.229804611038918</c:v>
+                  <c:v>0.365145211569558</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.22944798521126</c:v>
+                  <c:v>0.364713477080186</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.229160535290685</c:v>
+                  <c:v>0.364344116476411</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.22891600396637</c:v>
+                  <c:v>0.364023237238352</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.228787986061699</c:v>
+                  <c:v>0.363740933886453</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.22880419424667</c:v>
+                  <c:v>0.363489937506877</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.229092214397264</c:v>
+                  <c:v>0.363264782254078</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.229563117108445</c:v>
+                  <c:v>0.363061270288603</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.230831343608773</c:v>
+                  <c:v>0.362876117155491</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.233148267242943</c:v>
+                  <c:v>0.362706710365757</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.235115660793098</c:v>
+                  <c:v>0.362550941185391</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.237081370453861</c:v>
+                  <c:v>0.362407084998469</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0.238393575925638</c:v>
+                  <c:v>0.362273714628085</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>0.238959528611999</c:v>
+                  <c:v>0.362149636468458</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>0.238683950348838</c:v>
+                  <c:v>0.362033842692052</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>0.23739560179741</c:v>
+                  <c:v>0.36192547497298</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>0.236542579629556</c:v>
+                  <c:v>0.361823796587286</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>0.234626610898862</c:v>
+                  <c:v>0.36172817069317</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>0.233995435653727</c:v>
+                  <c:v>0.361638043230761</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>0.231828774954068</c:v>
+                  <c:v>0.361552929317659</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>0.231759069078184</c:v>
+                  <c:v>0.361472402320379</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>0.231433154455362</c:v>
+                  <c:v>0.361396084996153</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>0.22986646056027</c:v>
+                  <c:v>0.361323642252776</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>0.230044834319485</c:v>
+                  <c:v>0.361254775184879</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>0.229941972318103</c:v>
+                  <c:v>0.361189216126051</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>0.23014043403052</c:v>
+                  <c:v>0.361126724516127</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>0.230240421662151</c:v>
+                  <c:v>0.361067083427636</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>0.230312207094358</c:v>
+                  <c:v>0.361010096629157</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>0.230353492005041</c:v>
+                  <c:v>0.360955586088985</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>0.23033132311013</c:v>
+                  <c:v>0.360903389842191</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>0.229854276445379</c:v>
+                  <c:v>0.360853360159398</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>0.230573207243521</c:v>
+                  <c:v>0.36080536196749</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>0.229939824855008</c:v>
+                  <c:v>0.360759271481811</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>0.229709925324083</c:v>
+                  <c:v>0.360714975016784</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>0.229916436640838</c:v>
+                  <c:v>0.360672367947764</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>0.230051666818479</c:v>
+                  <c:v>0.360631353801669</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>0.230271967426747</c:v>
+                  <c:v>0.360591843457734</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>0.230808713631644</c:v>
+                  <c:v>0.360553754442779</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>0.231629571975237</c:v>
+                  <c:v>0.360517010307969</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>0.23240248647239</c:v>
+                  <c:v>0.360481540076009</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>0.232699948855421</c:v>
+                  <c:v>0.360447277749513</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>0.231806695266302</c:v>
+                  <c:v>0.360414161872603</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>0.231879423844041</c:v>
+                  <c:v>0.360382135139023</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>0.231928405813462</c:v>
+                  <c:v>0.360351144040986</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>0.23158021781723</c:v>
+                  <c:v>0.36032113855382</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>0.23135429060547</c:v>
+                  <c:v>0.360292071852134</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>0.230883579010857</c:v>
+                  <c:v>0.360263900053831</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>0.230235545620962</c:v>
+                  <c:v>0.360236581988775</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>0.230217487727037</c:v>
+                  <c:v>0.360210078989332</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>0.229965288926331</c:v>
+                  <c:v>0.360184354700378</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>0.230114476755613</c:v>
+                  <c:v>0.360159374906653</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>0.230089540773493</c:v>
+                  <c:v>0.360135107375603</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>0.229530084953307</c:v>
+                  <c:v>0.360111521714119</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3157,212 +3157,212 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="61"/>
                 <c:pt idx="0">
-                  <c:v>0.0645013850167206</c:v>
+                  <c:v>0.323952370964491</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.0594602817249425</c:v>
+                  <c:v>0.141892044975742</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.0569668476197837</c:v>
+                  <c:v>0.138300520864452</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.0557055184179631</c:v>
+                  <c:v>0.136588939873614</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.054666627199334</c:v>
+                  <c:v>0.135510033009632</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.0540041392699339</c:v>
+                  <c:v>0.13474564201022</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.0534665307002028</c:v>
+                  <c:v>0.134166165325115</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.0530655955994813</c:v>
+                  <c:v>0.133706870144534</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.0528101592547487</c:v>
+                  <c:v>0.133331025532177</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.0526463779175069</c:v>
+                  <c:v>0.133015920363919</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.0525145509347133</c:v>
+                  <c:v>0.132746635210976</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.0524025368719315</c:v>
+                  <c:v>0.132512917249489</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.0523439425661684</c:v>
+                  <c:v>0.132307466984589</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.0523513593048682</c:v>
+                  <c:v>0.132124934668753</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.0524832426974421</c:v>
+                  <c:v>0.131961302026102</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.0526992247365456</c:v>
+                  <c:v>0.131813485983574</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.0532831091922315</c:v>
+                  <c:v>0.131679076401845</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.0543581145183869</c:v>
+                  <c:v>0.131556157744349</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.0552793739501751</c:v>
+                  <c:v>0.131443184954413</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.0562075762162812</c:v>
+                  <c:v>0.131338895257088</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0.0568314970426131</c:v>
+                  <c:v>0.131242244310431</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>0.0571016563144691</c:v>
+                  <c:v>0.131152359194236</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>0.0569700281541266</c:v>
+                  <c:v>0.131068503254373</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>0.0563566717527544</c:v>
+                  <c:v>0.130990049434417</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>0.0559523919778049</c:v>
+                  <c:v>0.130916459776837</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>0.0550496465418862</c:v>
+                  <c:v>0.130847269473027</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>0.0547538639067777</c:v>
+                  <c:v>0.130782074311773</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>0.0537445808967039</c:v>
+                  <c:v>0.13072052069818</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>0.0537122660999865</c:v>
+                  <c:v>0.130662297639266</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>0.0535613049811598</c:v>
+                  <c:v>0.130607130250547</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>0.0528385896905065</c:v>
+                  <c:v>0.130554774450812</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>0.0529206257970793</c:v>
+                  <c:v>0.130505012593877</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>0.0528733106335395</c:v>
+                  <c:v>0.130457649845751</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>0.0529646193757562</c:v>
+                  <c:v>0.130412511159747</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>0.0530106517671655</c:v>
+                  <c:v>0.13036943873494</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>0.0530437127366745</c:v>
+                  <c:v>0.130328289868193</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>0.0530627312789166</c:v>
+                  <c:v>0.130288935128842</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>0.0530525184056635</c:v>
+                  <c:v>0.130251256799584</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>0.0528329884002288</c:v>
+                  <c:v>0.130215147538328</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>0.0531640038985637</c:v>
+                  <c:v>0.130180509224491</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>0.0528723230543521</c:v>
+                  <c:v>0.130147251960087</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>0.0527666497923961</c:v>
+                  <c:v>0.130115293201359</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>0.0528615678376205</c:v>
+                  <c:v>0.130084557001047</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>0.0529237694059606</c:v>
+                  <c:v>0.130054973344825</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>0.0530251789825849</c:v>
+                  <c:v>0.130026477568246</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>0.0532726622882944</c:v>
+                  <c:v>0.129999009842784</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>0.0536522586134317</c:v>
+                  <c:v>0.129972514721396</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>0.0540109157185494</c:v>
+                  <c:v>0.129946940735571</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>0.0541492661973158</c:v>
+                  <c:v>0.129922240037034</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>0.0537343439702843</c:v>
+                  <c:v>0.129898368078331</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>0.0537680672022446</c:v>
+                  <c:v>0.129875283327361</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>0.0537907854231743</c:v>
+                  <c:v>0.129852947011647</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>0.0536293972842757</c:v>
+                  <c:v>0.129831322888721</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>0.0535248077815605</c:v>
+                  <c:v>0.129810377039503</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>0.0533072270568627</c:v>
+                  <c:v>0.129790077681997</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>0.0530084064673824</c:v>
+                  <c:v>0.129770395002955</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>0.0530000916553484</c:v>
+                  <c:v>0.129751301005501</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>0.0528840341109711</c:v>
+                  <c:v>0.129732769370928</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>0.0529526724125096</c:v>
+                  <c:v>0.129714775333151</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>0.0529411967733571</c:v>
+                  <c:v>0.129697295564437</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>0.0526840598986724</c:v>
+                  <c:v>0.129680308071258</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="309699736"/>
-        <c:axId val="309689368"/>
+        <c:axId val="276873080"/>
+        <c:axId val="277629720"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="309699736"/>
+        <c:axId val="276873080"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="309689368"/>
+        <c:crossAx val="277629720"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="309689368"/>
+        <c:axId val="277629720"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3370,11 +3370,11 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="309699736"/>
+        <c:crossAx val="276873080"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
-        <c:majorUnit val="0.02"/>
-        <c:minorUnit val="0.002"/>
+        <c:majorUnit val="0.01"/>
+        <c:minorUnit val="0.001"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -3403,8 +3403,8 @@
     <xdr:to>
       <xdr:col>13</xdr:col>
       <xdr:colOff>609600</xdr:colOff>
-      <xdr:row>34</xdr:row>
-      <xdr:rowOff>25400</xdr:rowOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>60960</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3748,8 +3748,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
   <dimension ref="A1:I62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="125" workbookViewId="0">
-      <selection activeCell="K5" sqref="K5"/>
+    <sheetView tabSelected="1" topLeftCell="B21" zoomScale="125" workbookViewId="0">
+      <selection activeCell="D51" sqref="D51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -3785,28 +3785,28 @@
     </row>
     <row r="2" spans="1:9">
       <c r="A2">
-        <v>0.32220770160606099</v>
+        <v>0.170891063275283</v>
       </c>
       <c r="B2">
-        <v>0.10381780297426001</v>
+        <v>2.9203755507357099E-2</v>
       </c>
       <c r="C2">
-        <v>0.27168019428478002</v>
+        <v>0.248586037714733</v>
       </c>
       <c r="D2">
-        <v>7.3810127966616207E-2</v>
+        <v>6.1795018146710803E-2</v>
       </c>
       <c r="E2">
-        <v>0.27929122899999997</v>
+        <v>0.16924127598843899</v>
       </c>
       <c r="F2">
-        <v>7.8003589999999998E-2</v>
+        <v>2.8642609498194901E-2</v>
       </c>
       <c r="G2">
-        <v>0.25397122871837302</v>
+        <v>0.56916813944957501</v>
       </c>
       <c r="H2">
-        <v>6.4501385016720605E-2</v>
+        <v>0.32395237096449098</v>
       </c>
       <c r="I2">
         <v>0</v>
@@ -3814,28 +3814,28 @@
     </row>
     <row r="3" spans="1:9">
       <c r="A3">
-        <v>0.246610098429972</v>
+        <v>0.17673462449434599</v>
       </c>
       <c r="B3">
-        <v>6.0816540647640603E-2</v>
+        <v>3.12351274951576E-2</v>
       </c>
       <c r="C3">
-        <v>0.22474805963550001</v>
+        <v>0.18727705278145301</v>
       </c>
       <c r="D3">
-        <v>5.0511690309922502E-2</v>
+        <v>3.5072694498507397E-2</v>
       </c>
       <c r="E3">
-        <v>0.22425267800000001</v>
+        <v>0.15697300151573801</v>
       </c>
       <c r="F3">
-        <v>5.0289264E-2</v>
+        <v>2.4640523204860099E-2</v>
       </c>
       <c r="G3">
-        <v>0.24384479023539199</v>
+        <v>0.376685604948931</v>
       </c>
       <c r="H3">
-        <v>5.9460281724942499E-2</v>
+        <v>0.14189204497574201</v>
       </c>
       <c r="I3">
         <v>500</v>
@@ -3843,28 +3843,28 @@
     </row>
     <row r="4" spans="1:9">
       <c r="A4">
-        <v>0.24437120869896201</v>
+        <v>0.189655529393182</v>
       </c>
       <c r="B4">
-        <v>5.9717287640991899E-2</v>
+        <v>3.5969219829408303E-2</v>
       </c>
       <c r="C4">
-        <v>0.221983970434628</v>
+        <v>0.182877923234987</v>
       </c>
       <c r="D4">
-        <v>4.9276883129921803E-2</v>
+        <v>3.3444334806741999E-2</v>
       </c>
       <c r="E4">
-        <v>0.20982408399999999</v>
+        <v>0.155885720566241</v>
       </c>
       <c r="F4">
-        <v>4.4026146000000002E-2</v>
+        <v>2.4300357876456399E-2</v>
       </c>
       <c r="G4">
-        <v>0.23867728760773099</v>
+        <v>0.37188777993428601</v>
       </c>
       <c r="H4">
-        <v>5.6966847619783698E-2</v>
+        <v>0.13830052086445199</v>
       </c>
       <c r="I4">
         <v>1000</v>
@@ -3872,28 +3872,28 @@
     </row>
     <row r="5" spans="1:9">
       <c r="A5">
-        <v>0.24307133658798999</v>
+        <v>0.19026908846872301</v>
       </c>
       <c r="B5">
-        <v>5.9083674670672298E-2</v>
+        <v>3.6202326026718801E-2</v>
       </c>
       <c r="C5">
-        <v>0.22416943564181899</v>
+        <v>0.18054154492699301</v>
       </c>
       <c r="D5">
-        <v>5.0251935875971897E-2</v>
+        <v>3.2595249444625399E-2</v>
       </c>
       <c r="E5">
-        <v>0.19414990400000001</v>
+        <v>0.156287576358033</v>
       </c>
       <c r="F5">
-        <v>3.7694184999999998E-2</v>
+        <v>2.44258065238682E-2</v>
       </c>
       <c r="G5">
-        <v>0.23602016527823</v>
+        <v>0.36957940942862899</v>
       </c>
       <c r="H5">
-        <v>5.5705518417963097E-2</v>
+        <v>0.13658893987361401</v>
       </c>
       <c r="I5">
         <v>1500</v>
@@ -3901,28 +3901,28 @@
     </row>
     <row r="6" spans="1:9">
       <c r="A6">
-        <v>0.24197034423956601</v>
+        <v>0.18579585650666</v>
       </c>
       <c r="B6">
-        <v>5.8549647491414197E-2</v>
+        <v>3.4520100295043599E-2</v>
       </c>
       <c r="C6">
-        <v>0.22945018878137399</v>
+        <v>0.17899222002562301</v>
       </c>
       <c r="D6">
-        <v>5.2647389131808199E-2</v>
+        <v>3.2038214829701199E-2</v>
       </c>
       <c r="E6">
-        <v>0.18821420799999999</v>
+        <v>0.15653965548818699</v>
       </c>
       <c r="F6">
-        <v>3.5424588E-2</v>
+        <v>2.4504663740360401E-2</v>
       </c>
       <c r="G6">
-        <v>0.233808954489202</v>
+        <v>0.36811687411694699</v>
       </c>
       <c r="H6">
-        <v>5.4666627199334003E-2</v>
+        <v>0.13551003300963199</v>
       </c>
       <c r="I6">
         <v>2000</v>
@@ -3930,28 +3930,28 @@
     </row>
     <row r="7" spans="1:9">
       <c r="A7">
-        <v>0.241020385863951</v>
+        <v>0.18276551732269899</v>
       </c>
       <c r="B7">
-        <v>5.8090826402008001E-2</v>
+        <v>3.3403234322234E-2</v>
       </c>
       <c r="C7">
-        <v>0.233198878993336</v>
+        <v>0.177875833951677</v>
       </c>
       <c r="D7">
-        <v>5.4381717163748802E-2</v>
+        <v>3.1639812304004797E-2</v>
       </c>
       <c r="E7">
-        <v>0.185115165</v>
+        <v>0.15674629853265901</v>
       </c>
       <c r="F7">
-        <v>3.4267623999999997E-2</v>
+        <v>2.4569402103689599E-2</v>
       </c>
       <c r="G7">
-        <v>0.23238790689262201</v>
+        <v>0.36707716083981601</v>
       </c>
       <c r="H7">
-        <v>5.4004139269933901E-2</v>
+        <v>0.13474564201021999</v>
       </c>
       <c r="I7">
         <v>2500</v>
@@ -3959,28 +3959,28 @@
     </row>
     <row r="8" spans="1:9">
       <c r="A8">
-        <v>0.24016118291268099</v>
+        <v>0.179319716808685</v>
       </c>
       <c r="B8">
-        <v>5.7677393778018303E-2</v>
+        <v>3.21555608363472E-2</v>
       </c>
       <c r="C8">
-        <v>0.23493700356231301</v>
+        <v>0.17703874597736999</v>
       </c>
       <c r="D8">
-        <v>5.5195395642838499E-2</v>
+        <v>3.1342717577239797E-2</v>
       </c>
       <c r="E8">
-        <v>0.18316126199999999</v>
+        <v>0.15694676442764599</v>
       </c>
       <c r="F8">
-        <v>3.3548047999999997E-2</v>
+        <v>2.4632286864307001E-2</v>
       </c>
       <c r="G8">
-        <v>0.23122830860472601</v>
+        <v>0.36628699857504499</v>
       </c>
       <c r="H8">
-        <v>5.3466530700202797E-2</v>
+        <v>0.13416616532511499</v>
       </c>
       <c r="I8">
         <v>3000</v>
@@ -3988,28 +3988,28 @@
     </row>
     <row r="9" spans="1:9">
       <c r="A9">
-        <v>0.23935962592486801</v>
+        <v>0.174464241845423</v>
       </c>
       <c r="B9">
-        <v>5.7293030522893099E-2</v>
+        <v>3.04377716826984E-2</v>
       </c>
       <c r="C9">
-        <v>0.235550044802046</v>
+        <v>0.17639595229593699</v>
       </c>
       <c r="D9">
-        <v>5.5483823606246201E-2</v>
+        <v>3.11155319863906E-2</v>
       </c>
       <c r="E9">
-        <v>0.181809368</v>
+        <v>0.15711398695384399</v>
       </c>
       <c r="F9">
-        <v>3.3054646E-2</v>
+        <v>2.4684804896532901E-2</v>
       </c>
       <c r="G9">
-        <v>0.23035970914958401</v>
+        <v>0.36565950027933602</v>
       </c>
       <c r="H9">
-        <v>5.3065595599481298E-2</v>
+        <v>0.133706870144534</v>
       </c>
       <c r="I9">
         <v>3500</v>
@@ -4017,28 +4017,28 @@
     </row>
     <row r="10" spans="1:9">
       <c r="A10">
-        <v>0.23859843444191101</v>
+        <v>0.17080213346254799</v>
       </c>
       <c r="B10">
-        <v>5.6929212918131099E-2</v>
+        <v>2.91733687953581E-2</v>
       </c>
       <c r="C10">
-        <v>0.23561062942366401</v>
+        <v>0.17589368939295499</v>
       </c>
       <c r="D10">
-        <v>5.55123686974155E-2</v>
+        <v>3.0938589968265501E-2</v>
       </c>
       <c r="E10">
-        <v>0.180824552</v>
+        <v>0.157234787280885</v>
       </c>
       <c r="F10">
-        <v>3.2697519000000001E-2</v>
+        <v>2.4722778331265099E-2</v>
       </c>
       <c r="G10">
-        <v>0.229804611038918</v>
+        <v>0.36514521156955798</v>
       </c>
       <c r="H10">
-        <v>5.2810159254748697E-2</v>
+        <v>0.13333102553217699</v>
       </c>
       <c r="I10">
         <v>4000</v>
@@ -4046,28 +4046,28 @@
     </row>
     <row r="11" spans="1:9">
       <c r="A11">
-        <v>0.23786819871641299</v>
+        <v>0.168570445993694</v>
       </c>
       <c r="B11">
-        <v>5.6581279960591202E-2</v>
+        <v>2.8415995262513101E-2</v>
       </c>
       <c r="C11">
-        <v>0.23538902874478901</v>
+        <v>0.17549547648678099</v>
       </c>
       <c r="D11">
-        <v>5.5407994853415403E-2</v>
+        <v>3.0798662267322599E-2</v>
       </c>
       <c r="E11">
-        <v>0.18008468499999999</v>
+        <v>0.157290948761065</v>
       </c>
       <c r="F11">
-        <v>3.2430493999999997E-2</v>
+        <v>2.47404425621559E-2</v>
       </c>
       <c r="G11">
-        <v>0.22944798521126</v>
+        <v>0.36471347708018598</v>
       </c>
       <c r="H11">
-        <v>5.2646377917506898E-2</v>
+        <v>0.13301592036391899</v>
       </c>
       <c r="I11">
         <v>4500</v>
@@ -4075,28 +4075,28 @@
     </row>
     <row r="12" spans="1:9">
       <c r="A12">
-        <v>0.237163442524114</v>
+        <v>0.16761287802952399</v>
       </c>
       <c r="B12">
-        <v>5.6246498469888703E-2</v>
+        <v>2.8094076881340298E-2</v>
       </c>
       <c r="C12">
-        <v>0.23464597418753699</v>
+        <v>0.17517565137372901</v>
       </c>
       <c r="D12">
-        <v>5.5058733202418497E-2</v>
+        <v>3.06865088342104E-2</v>
       </c>
       <c r="E12">
-        <v>0.17951825599999999</v>
+        <v>0.157237667018754</v>
       </c>
       <c r="F12">
-        <v>3.2226803999999998E-2</v>
+        <v>2.4723683929500601E-2</v>
       </c>
       <c r="G12">
-        <v>0.229160535290685</v>
+        <v>0.36434411647641102</v>
       </c>
       <c r="H12">
-        <v>5.25145509347133E-2</v>
+        <v>0.13274663521097599</v>
       </c>
       <c r="I12">
         <v>5000</v>
@@ -4104,28 +4104,28 @@
     </row>
     <row r="13" spans="1:9">
       <c r="A13">
-        <v>0.236480717977958</v>
+        <v>0.16709523710390201</v>
       </c>
       <c r="B13">
-        <v>5.5923129975370703E-2</v>
+        <v>2.7920818262809399E-2</v>
       </c>
       <c r="C13">
-        <v>0.23347118772067299</v>
+        <v>0.17491579593200399</v>
       </c>
       <c r="D13">
-        <v>5.4508795495702103E-2</v>
+        <v>3.0595535666526601E-2</v>
       </c>
       <c r="E13">
-        <v>0.179079816</v>
+        <v>0.15709747772135499</v>
       </c>
       <c r="F13">
-        <v>3.2069581E-2</v>
+        <v>2.4679617506411702E-2</v>
       </c>
       <c r="G13">
-        <v>0.22891600396636999</v>
+        <v>0.364023237238352</v>
       </c>
       <c r="H13">
-        <v>5.2402536871931499E-2</v>
+        <v>0.13251291724948899</v>
       </c>
       <c r="I13">
         <v>5500</v>
@@ -4133,28 +4133,28 @@
     </row>
     <row r="14" spans="1:9">
       <c r="A14">
-        <v>0.23581766553943201</v>
+        <v>0.16683949641070001</v>
       </c>
       <c r="B14">
-        <v>5.5609971380467499E-2</v>
+        <v>2.7835417562576101E-2</v>
       </c>
       <c r="C14">
-        <v>0.232288453903818</v>
+        <v>0.17470250409354199</v>
       </c>
       <c r="D14">
-        <v>5.3957925817026499E-2</v>
+        <v>3.05209649365542E-2</v>
       </c>
       <c r="E14">
-        <v>0.17873871199999999</v>
+        <v>0.15695010810187099</v>
       </c>
       <c r="F14">
-        <v>3.1947527000000003E-2</v>
+        <v>2.4633336433189101E-2</v>
       </c>
       <c r="G14">
-        <v>0.22878798606169901</v>
+        <v>0.36374093388645301</v>
       </c>
       <c r="H14">
-        <v>5.2343942566168401E-2</v>
+        <v>0.13230746698458901</v>
       </c>
       <c r="I14">
         <v>6000</v>
@@ -4162,28 +4162,28 @@
     </row>
     <row r="15" spans="1:9">
       <c r="A15">
-        <v>0.23517254275079699</v>
+        <v>0.16666677243660699</v>
       </c>
       <c r="B15">
-        <v>5.5306124863875802E-2</v>
+        <v>2.77778130344359E-2</v>
       </c>
       <c r="C15">
-        <v>0.231141803118564</v>
+        <v>0.17452589500013299</v>
       </c>
       <c r="D15">
-        <v>5.3426533148901001E-2</v>
+        <v>3.0459288025597501E-2</v>
       </c>
       <c r="E15">
-        <v>0.17847332099999999</v>
+        <v>0.15677534279376901</v>
       </c>
       <c r="F15">
-        <v>3.1852725999999998E-2</v>
+        <v>2.4578508108104E-2</v>
       </c>
       <c r="G15">
-        <v>0.22880419424667001</v>
+        <v>0.36348993750687703</v>
       </c>
       <c r="H15">
-        <v>5.23513593048682E-2</v>
+        <v>0.132124934668753</v>
       </c>
       <c r="I15">
         <v>6500</v>
@@ -4191,28 +4191,28 @@
     </row>
     <row r="16" spans="1:9">
       <c r="A16">
-        <v>0.23454398721530401</v>
+        <v>0.16651451439894599</v>
       </c>
       <c r="B16">
-        <v>5.5010881938852903E-2</v>
+        <v>2.7727083505516899E-2</v>
       </c>
       <c r="C16">
-        <v>0.23003517562713399</v>
+        <v>0.17437859397668401</v>
       </c>
       <c r="D16">
-        <v>5.2916182025806599E-2</v>
+        <v>3.0407894037285398E-2</v>
       </c>
       <c r="E16">
-        <v>0.17826784700000001</v>
+        <v>0.156479924462197</v>
       </c>
       <c r="F16">
-        <v>3.1779425E-2</v>
+        <v>2.4485966759694899E-2</v>
       </c>
       <c r="G16">
-        <v>0.22909221439726399</v>
+        <v>0.36326478225407799</v>
       </c>
       <c r="H16">
-        <v>5.2483242697442103E-2</v>
+        <v>0.13196130202610201</v>
       </c>
       <c r="I16">
         <v>7000</v>
@@ -4220,28 +4220,28 @@
     </row>
     <row r="17" spans="1:9">
       <c r="A17">
-        <v>0.23393089898078701</v>
+        <v>0.16636592861863</v>
       </c>
       <c r="B17">
-        <v>5.4723665497959401E-2</v>
+        <v>2.7677622205139099E-2</v>
       </c>
       <c r="C17">
-        <v>0.228970645773965</v>
+        <v>0.174255025486758</v>
       </c>
       <c r="D17">
-        <v>5.2427556626146801E-2</v>
+        <v>3.0364813907390702E-2</v>
       </c>
       <c r="E17">
-        <v>0.17811042199999999</v>
+        <v>0.15610085489730099</v>
       </c>
       <c r="F17">
-        <v>3.1723321999999998E-2</v>
+        <v>2.4367476899668301E-2</v>
       </c>
       <c r="G17">
-        <v>0.22956311710844499</v>
+        <v>0.36306127028860302</v>
       </c>
       <c r="H17">
-        <v>5.2699224736545598E-2</v>
+        <v>0.13181348598357401</v>
       </c>
       <c r="I17">
         <v>7500</v>
@@ -4249,28 +4249,28 @@
     </row>
     <row r="18" spans="1:9">
       <c r="A18">
-        <v>0.23333238406215701</v>
+        <v>0.16620033115400201</v>
       </c>
       <c r="B18">
-        <v>5.4444001452130103E-2</v>
+        <v>2.7622550075700102E-2</v>
       </c>
       <c r="C18">
-        <v>0.22794963924412701</v>
+        <v>0.174150918941337</v>
       </c>
       <c r="D18">
-        <v>5.1961038031527997E-2</v>
+        <v>3.0328542568112099E-2</v>
       </c>
       <c r="E18">
-        <v>0.177991923</v>
+        <v>0.155728108838255</v>
       </c>
       <c r="F18">
-        <v>3.1681124999999997E-2</v>
+        <v>2.4251243882339599E-2</v>
       </c>
       <c r="G18">
-        <v>0.230831343608773</v>
+        <v>0.36287611715549101</v>
       </c>
       <c r="H18">
-        <v>5.3283109192231497E-2</v>
+        <v>0.13167907640184501</v>
       </c>
       <c r="I18">
         <v>8000</v>
@@ -4278,28 +4278,28 @@
     </row>
     <row r="19" spans="1:9">
       <c r="A19">
-        <v>0.232747728404397</v>
+        <v>0.16597501441271501</v>
       </c>
       <c r="B19">
-        <v>5.4171505077407298E-2</v>
+        <v>2.7547705409301002E-2</v>
       </c>
       <c r="C19">
-        <v>0.22697301792058799</v>
+        <v>0.17406296085077</v>
       </c>
       <c r="D19">
-        <v>5.1516750863979499E-2</v>
+        <v>3.0297914340136699E-2</v>
       </c>
       <c r="E19">
-        <v>0.17790520500000001</v>
+        <v>0.155255506279528</v>
       </c>
       <c r="F19">
-        <v>3.1650261999999998E-2</v>
+        <v>2.4104272230112599E-2</v>
       </c>
       <c r="G19">
-        <v>0.23314826724294299</v>
+        <v>0.36270671036575702</v>
       </c>
       <c r="H19">
-        <v>5.4358114518386902E-2</v>
+        <v>0.13155615774434901</v>
       </c>
       <c r="I19">
         <v>8500</v>
@@ -4307,28 +4307,28 @@
     </row>
     <row r="20" spans="1:9">
       <c r="A20">
-        <v>0.232176385224999</v>
+        <v>0.16559732919558801</v>
       </c>
       <c r="B20">
-        <v>5.3905873856147202E-2</v>
+        <v>2.7422475436712099E-2</v>
       </c>
       <c r="C20">
-        <v>0.22604114165290601</v>
+        <v>0.173988547995724</v>
       </c>
       <c r="D20">
-        <v>5.1094597719749502E-2</v>
+        <v>3.0272014833660599E-2</v>
       </c>
       <c r="E20">
-        <v>0.177844577</v>
+        <v>0.15576678690287399</v>
       </c>
       <c r="F20">
-        <v>3.1628692999999999E-2</v>
+        <v>2.4263291902045299E-2</v>
       </c>
       <c r="G20">
-        <v>0.23511566079309801</v>
+        <v>0.362550941185391</v>
       </c>
       <c r="H20">
-        <v>5.5279373950175098E-2</v>
+        <v>0.13144318495441301</v>
       </c>
       <c r="I20">
         <v>9000</v>
@@ -4336,28 +4336,28 @@
     </row>
     <row r="21" spans="1:9">
       <c r="A21">
-        <v>0.23161796547952801</v>
+        <v>0.16487500365987201</v>
       </c>
       <c r="B21">
-        <v>5.3646881932876103E-2</v>
+        <v>2.7183766831842902E-2</v>
       </c>
       <c r="C21">
-        <v>0.225153933428061</v>
+        <v>0.173925610651012</v>
       </c>
       <c r="D21">
-        <v>5.0694293738127699E-2</v>
+        <v>3.0250118040327598E-2</v>
       </c>
       <c r="E21">
-        <v>0.17780545</v>
+        <v>0.15767878584245201</v>
       </c>
       <c r="F21">
-        <v>3.1614778000000003E-2</v>
+        <v>2.4862599504750001E-2</v>
       </c>
       <c r="G21">
-        <v>0.23708137045386099</v>
+        <v>0.36240708499846902</v>
       </c>
       <c r="H21">
-        <v>5.6207576216281203E-2</v>
+        <v>0.131338895257088</v>
       </c>
       <c r="I21">
         <v>9500</v>
@@ -4365,28 +4365,28 @@
     </row>
     <row r="22" spans="1:9">
       <c r="A22">
-        <v>0.231072224738051</v>
+        <v>0.163513597041372</v>
       </c>
       <c r="B22">
-        <v>5.33943730453924E-2</v>
+        <v>2.6736696417408098E-2</v>
       </c>
       <c r="C22">
-        <v>0.224310945291502</v>
+        <v>0.17387248469370301</v>
       </c>
       <c r="D22">
-        <v>5.0315400177567401E-2</v>
+        <v>3.02316409335622E-2</v>
       </c>
       <c r="E22">
-        <v>0.17778408000000001</v>
+        <v>0.15909211723041999</v>
       </c>
       <c r="F22">
-        <v>3.1607178999999999E-2</v>
+        <v>2.5310301764857698E-2</v>
       </c>
       <c r="G22">
-        <v>0.23839357592563801</v>
+        <v>0.362273714628085</v>
       </c>
       <c r="H22">
-        <v>5.6831497042613102E-2</v>
+        <v>0.13124224431043099</v>
       </c>
       <c r="I22">
         <v>10000</v>
@@ -4394,28 +4394,28 @@
     </row>
     <row r="23" spans="1:9">
       <c r="A23">
-        <v>0.230539041984793</v>
+        <v>0.16143262539269099</v>
       </c>
       <c r="B23">
-        <v>5.3148249879266397E-2</v>
+        <v>2.60604925411769E-2</v>
       </c>
       <c r="C23">
-        <v>0.223511422268519</v>
+        <v>0.17382781809271999</v>
       </c>
       <c r="D23">
-        <v>4.99573558844962E-2</v>
+        <v>3.0216110342875999E-2</v>
       </c>
       <c r="E23">
-        <v>0.17777737900000001</v>
+        <v>0.16043174862704701</v>
       </c>
       <c r="F23">
-        <v>3.1604795999999998E-2</v>
+        <v>2.5738345967532002E-2</v>
       </c>
       <c r="G23">
-        <v>0.23895952861199901</v>
+        <v>0.36214963646845799</v>
       </c>
       <c r="H23">
-        <v>5.7101656314469097E-2</v>
+        <v>0.13115235919423601</v>
       </c>
       <c r="I23">
         <v>10500</v>
@@ -4423,28 +4423,28 @@
     </row>
     <row r="24" spans="1:9">
       <c r="A24">
-        <v>0.23001838786971901</v>
+        <v>0.15928355263288199</v>
       </c>
       <c r="B24">
-        <v>5.2908458758184597E-2</v>
+        <v>2.5371250139352299E-2</v>
       </c>
       <c r="C24">
-        <v>0.22275436224485201</v>
+        <v>0.17379050179910899</v>
       </c>
       <c r="D24">
-        <v>4.9619505899111002E-2</v>
+        <v>3.02031385155863E-2</v>
       </c>
       <c r="E24">
-        <v>0.177782781</v>
+        <v>0.16124705934144401</v>
       </c>
       <c r="F24">
-        <v>3.1606716999999999E-2</v>
+        <v>2.6000614146263298E-2</v>
       </c>
       <c r="G24">
-        <v>0.23868395034883799</v>
+        <v>0.36203384269205202</v>
       </c>
       <c r="H24">
-        <v>5.6970028154126599E-2</v>
+        <v>0.131068503254373</v>
       </c>
       <c r="I24">
         <v>11000</v>
@@ -4452,28 +4452,28 @@
     </row>
     <row r="25" spans="1:9">
       <c r="A25">
-        <v>0.22951028230964399</v>
+        <v>0.15783284586124199</v>
       </c>
       <c r="B25">
-        <v>5.2674969685852502E-2</v>
+        <v>2.4911207232658699E-2</v>
       </c>
       <c r="C25">
-        <v>0.22203857043415801</v>
+        <v>0.17375961812340199</v>
       </c>
       <c r="D25">
-        <v>4.9301126760444798E-2</v>
+        <v>3.01924048903905E-2</v>
       </c>
       <c r="E25">
-        <v>0.17779813999999999</v>
+        <v>0.16119245960166501</v>
       </c>
       <c r="F25">
-        <v>3.1612177999999998E-2</v>
+        <v>2.5983009032434601E-2</v>
       </c>
       <c r="G25">
-        <v>0.23739560179741001</v>
+        <v>0.36192547497298</v>
       </c>
       <c r="H25">
-        <v>5.6356671752754398E-2</v>
+        <v>0.130990049434417</v>
       </c>
       <c r="I25">
         <v>11500</v>
@@ -4481,28 +4481,28 @@
     </row>
     <row r="26" spans="1:9">
       <c r="A26">
-        <v>0.22901474410828401</v>
+        <v>0.15708808323590601</v>
       </c>
       <c r="B26">
-        <v>5.2447753018982801E-2</v>
+        <v>2.4676665894731099E-2</v>
       </c>
       <c r="C26">
-        <v>0.22136270763868399</v>
+        <v>0.173734401772807</v>
       </c>
       <c r="D26">
-        <v>4.9001448333129798E-2</v>
+        <v>3.0183642359355101E-2</v>
       </c>
       <c r="E26">
-        <v>0.177821643</v>
+        <v>0.15944504818859501</v>
       </c>
       <c r="F26">
-        <v>3.1620536999999997E-2</v>
+        <v>2.5422723391863598E-2</v>
       </c>
       <c r="G26">
-        <v>0.23654257962955599</v>
+        <v>0.36182379658728597</v>
       </c>
       <c r="H26">
-        <v>5.5952391977804897E-2</v>
+        <v>0.130916459776837</v>
       </c>
       <c r="I26">
         <v>12000</v>
@@ -4510,28 +4510,28 @@
     </row>
     <row r="27" spans="1:9">
       <c r="A27">
-        <v>0.22853173798573001</v>
+        <v>0.156736964206873</v>
       </c>
       <c r="B27">
-        <v>5.2226755266778301E-2</v>
+        <v>2.45664759487868E-2</v>
       </c>
       <c r="C27">
-        <v>0.22072533198720801</v>
+        <v>0.17371421014744801</v>
       </c>
       <c r="D27">
-        <v>4.8719672180863503E-2</v>
+        <v>3.0176626807151899E-2</v>
       </c>
       <c r="E27">
-        <v>0.177851759</v>
+        <v>0.15803822863541001</v>
       </c>
       <c r="F27">
-        <v>3.1631248000000001E-2</v>
+        <v>2.4976081710218201E-2</v>
       </c>
       <c r="G27">
-        <v>0.234626610898862</v>
+        <v>0.36172817069316998</v>
       </c>
       <c r="H27">
-        <v>5.5049646541886203E-2</v>
+        <v>0.13084726947302699</v>
       </c>
       <c r="I27">
         <v>12500</v>
@@ -4539,28 +4539,28 @@
     </row>
     <row r="28" spans="1:9">
       <c r="A28">
-        <v>0.22806112627466699</v>
+        <v>0.15656474877260901</v>
       </c>
       <c r="B28">
-        <v>5.2011877317669597E-2</v>
+        <v>2.4512520558230201E-2</v>
       </c>
       <c r="C28">
-        <v>0.22012493421075399</v>
+        <v>0.173698500477004</v>
       </c>
       <c r="D28">
-        <v>4.8454986661288703E-2</v>
+        <v>3.0171169067959702E-2</v>
       </c>
       <c r="E28">
-        <v>0.17788718100000001</v>
+        <v>0.157556503666126</v>
       </c>
       <c r="F28">
-        <v>3.1643849000000002E-2</v>
+        <v>2.4824051847493998E-2</v>
       </c>
       <c r="G28">
-        <v>0.23399543565372699</v>
+        <v>0.36163804323076099</v>
       </c>
       <c r="H28">
-        <v>5.4753863906777701E-2</v>
+        <v>0.13078207431177299</v>
       </c>
       <c r="I28">
         <v>13000</v>
@@ -4568,28 +4568,28 @@
     </row>
     <row r="29" spans="1:9">
       <c r="A29">
-        <v>0.22760263276821099</v>
+        <v>0.15647099879605</v>
       </c>
       <c r="B29">
-        <v>5.1802958443021199E-2</v>
+        <v>2.4483173464233701E-2</v>
       </c>
       <c r="C29">
-        <v>0.21955996679778</v>
+        <v>0.17368681206081699</v>
       </c>
       <c r="D29">
-        <v>4.8206579020242203E-2</v>
+        <v>3.0167108683849898E-2</v>
       </c>
       <c r="E29">
-        <v>0.177926793</v>
+        <v>0.157193905253803</v>
       </c>
       <c r="F29">
-        <v>3.1657944E-2</v>
+        <v>2.4709923848941599E-2</v>
       </c>
       <c r="G29">
-        <v>0.23182877495406801</v>
+        <v>0.36155292931765898</v>
       </c>
       <c r="H29">
-        <v>5.3744580896703899E-2</v>
+        <v>0.13072052069817999</v>
       </c>
       <c r="I29">
         <v>13500</v>
@@ -4597,28 +4597,28 @@
     </row>
     <row r="30" spans="1:9">
       <c r="A30">
-        <v>0.22715582448143901</v>
+        <v>0.156413260150052</v>
       </c>
       <c r="B30">
-        <v>5.1599768595842699E-2</v>
+        <v>2.4465107950767902E-2</v>
       </c>
       <c r="C30">
-        <v>0.219028867565015</v>
+        <v>0.17367875235201599</v>
       </c>
       <c r="D30">
-        <v>4.7973644826812802E-2</v>
+        <v>3.0164309018553201E-2</v>
       </c>
       <c r="E30">
-        <v>0.17796963599999999</v>
+        <v>0.15663572394039299</v>
       </c>
       <c r="F30">
-        <v>3.1673191000000003E-2</v>
+        <v>2.45347500143312E-2</v>
       </c>
       <c r="G30">
-        <v>0.231759069078184</v>
+        <v>0.36147240232037903</v>
       </c>
       <c r="H30">
-        <v>5.37122660999865E-2</v>
+        <v>0.13066229763926601</v>
       </c>
       <c r="I30">
         <v>14000</v>
@@ -4626,28 +4626,28 @@
     </row>
     <row r="31" spans="1:9">
       <c r="A31">
-        <v>0.22672011384141399</v>
+        <v>0.15637361580756501</v>
       </c>
       <c r="B31">
-        <v>5.1402010020264101E-2</v>
+        <v>2.44527077207322E-2</v>
       </c>
       <c r="C31">
-        <v>0.21853007829850299</v>
+        <v>0.173673985963677</v>
       </c>
       <c r="D31">
-        <v>4.77553951211502E-2</v>
+        <v>3.0162653400511798E-2</v>
       </c>
       <c r="E31">
-        <v>0.17801488500000001</v>
+        <v>0.15598465482402099</v>
       </c>
       <c r="F31">
-        <v>3.1689298999999997E-2</v>
+        <v>2.4331212540569001E-2</v>
       </c>
       <c r="G31">
-        <v>0.231433154455362</v>
+        <v>0.361396084996153</v>
       </c>
       <c r="H31">
-        <v>5.3561304981159803E-2</v>
+        <v>0.13060713025054699</v>
       </c>
       <c r="I31">
         <v>14500</v>
@@ -4655,28 +4655,28 @@
     </row>
     <row r="32" spans="1:9">
       <c r="A32">
-        <v>0.22629478007006601</v>
+        <v>0.156344144680854</v>
       </c>
       <c r="B32">
-        <v>5.1209327486959701E-2</v>
+        <v>2.4443491575988002E-2</v>
       </c>
       <c r="C32">
-        <v>0.218062059172906</v>
+        <v>0.173672225916043</v>
       </c>
       <c r="D32">
-        <v>4.7551061650728303E-2</v>
+        <v>3.01620420546331E-2</v>
       </c>
       <c r="E32">
-        <v>0.17806182600000001</v>
+        <v>0.15543324349639301</v>
       </c>
       <c r="F32">
-        <v>3.1706013999999998E-2</v>
+        <v>2.4159493183809101E-2</v>
       </c>
       <c r="G32">
-        <v>0.22986646056026999</v>
+        <v>0.36132364225277602</v>
       </c>
       <c r="H32">
-        <v>5.2838589690506498E-2</v>
+        <v>0.13055477445081201</v>
       </c>
       <c r="I32">
         <v>15000</v>
@@ -4684,28 +4684,28 @@
     </row>
     <row r="33" spans="1:9">
       <c r="A33">
-        <v>0.22587900540811801</v>
+        <v>0.15632106248768299</v>
       </c>
       <c r="B33">
-        <v>5.1021325084160997E-2</v>
+        <v>2.4436274577278198E-2</v>
       </c>
       <c r="C33">
-        <v>0.217623299657416</v>
+        <v>0.17367322661745399</v>
       </c>
       <c r="D33">
-        <v>4.73599005537816E-2</v>
+        <v>3.0162389643717698E-2</v>
       </c>
       <c r="E33">
-        <v>0.17810983899999999</v>
+        <v>0.155035155721611</v>
       </c>
       <c r="F33">
-        <v>3.1723115000000003E-2</v>
+        <v>2.40358995096242E-2</v>
       </c>
       <c r="G33">
-        <v>0.230044834319485</v>
+        <v>0.36125477518487897</v>
       </c>
       <c r="H33">
-        <v>5.2920625797079297E-2</v>
+        <v>0.13050501259387701</v>
       </c>
       <c r="I33">
         <v>15500</v>
@@ -4713,28 +4713,28 @@
     </row>
     <row r="34" spans="1:9">
       <c r="A34">
-        <v>0.225471920097044</v>
+        <v>0.156302374631209</v>
       </c>
       <c r="B34">
-        <v>5.0837586752247803E-2</v>
+        <v>2.4430432315355001E-2</v>
       </c>
       <c r="C34">
-        <v>0.21721232657594899</v>
+        <v>0.173676778198121</v>
       </c>
       <c r="D34">
-        <v>4.7181194816536903E-2</v>
+        <v>3.0163623285279301E-2</v>
       </c>
       <c r="E34">
-        <v>0.178158384</v>
+        <v>0.15475178275410201</v>
       </c>
       <c r="F34">
-        <v>3.1740409999999997E-2</v>
+        <v>2.3948114265573001E-2</v>
       </c>
       <c r="G34">
-        <v>0.22994197231810301</v>
+        <v>0.36118921612605098</v>
       </c>
       <c r="H34">
-        <v>5.2873310633539498E-2</v>
+        <v>0.13045764984575101</v>
       </c>
       <c r="I34">
         <v>16000</v>
@@ -4742,28 +4742,28 @@
     </row>
     <row r="35" spans="1:9">
       <c r="A35">
-        <v>0.22507264982630201</v>
+        <v>0.156286913269957</v>
       </c>
       <c r="B35">
-        <v>5.0657697699833401E-2</v>
+        <v>2.4425599259451002E-2</v>
       </c>
       <c r="C35">
-        <v>0.216827709919856</v>
+        <v>0.17368270190884999</v>
       </c>
       <c r="D35">
-        <v>4.70142557890895E-2</v>
+        <v>3.0165680942358601E-2</v>
       </c>
       <c r="E35">
-        <v>0.17820699000000001</v>
+        <v>0.15454203158677601</v>
       </c>
       <c r="F35">
-        <v>3.1757730999999997E-2</v>
+        <v>2.3883239526968199E-2</v>
       </c>
       <c r="G35">
-        <v>0.23014043403052001</v>
+        <v>0.36112672451612698</v>
       </c>
       <c r="H35">
-        <v>5.2964619375756201E-2</v>
+        <v>0.130412511159747</v>
       </c>
       <c r="I35">
         <v>16500</v>
@@ -4771,28 +4771,28 @@
     </row>
     <row r="36" spans="1:9">
       <c r="A36">
-        <v>0.22468036030133701</v>
+        <v>0.15627392561043499</v>
       </c>
       <c r="B36">
-        <v>5.0481264305139002E-2</v>
+        <v>2.4421539825695799E-2</v>
       </c>
       <c r="C36">
-        <v>0.216468066924491</v>
+        <v>0.17369084636592799</v>
       </c>
       <c r="D36">
-        <v>4.68584239980262E-2</v>
+        <v>3.0168510111312601E-2</v>
       </c>
       <c r="E36">
-        <v>0.17825524100000001</v>
+        <v>0.15438333081553701</v>
       </c>
       <c r="F36">
-        <v>3.1774930999999999E-2</v>
+        <v>2.3834212833699801E-2</v>
       </c>
       <c r="G36">
-        <v>0.230240421662151</v>
+        <v>0.36106708342763599</v>
       </c>
       <c r="H36">
-        <v>5.3010651767165497E-2</v>
+        <v>0.13036943873494</v>
       </c>
       <c r="I36">
         <v>17000</v>
@@ -4800,28 +4800,28 @@
     </row>
     <row r="37" spans="1:9">
       <c r="A37">
-        <v>0.22429429512316101</v>
+        <v>0.156262887800976</v>
       </c>
       <c r="B37">
-        <v>5.0307930824795698E-2</v>
+        <v>2.4418090103900399E-2</v>
       </c>
       <c r="C37">
-        <v>0.21613206482725</v>
+        <v>0.173701084475269</v>
       </c>
       <c r="D37">
-        <v>4.6713069446490903E-2</v>
+        <v>3.0172066747884599E-2</v>
       </c>
       <c r="E37">
-        <v>0.178302768</v>
+        <v>0.15426430003606101</v>
       </c>
       <c r="F37">
-        <v>3.1791877000000003E-2</v>
+        <v>2.37974742656159E-2</v>
       </c>
       <c r="G37">
-        <v>0.23031220709435801</v>
+        <v>0.36101009662915701</v>
       </c>
       <c r="H37">
-        <v>5.3043712736674499E-2</v>
+        <v>0.130328289868193</v>
       </c>
       <c r="I37">
         <v>17500</v>
@@ -4829,28 +4829,28 @@
     </row>
     <row r="38" spans="1:9">
       <c r="A38">
-        <v>0.223913804779726</v>
+        <v>0.15625341475524901</v>
       </c>
       <c r="B38">
-        <v>5.0137391970933198E-2</v>
+        <v>2.4415129622676002E-2</v>
       </c>
       <c r="C38">
-        <v>0.21581842263204101</v>
+        <v>0.17371331090835401</v>
       </c>
       <c r="D38">
-        <v>4.6577591547382599E-2</v>
+        <v>3.01763143867427E-2</v>
       </c>
       <c r="E38">
-        <v>0.17834924499999999</v>
+        <v>0.15417854508427101</v>
       </c>
       <c r="F38">
-        <v>3.1808453E-2</v>
+        <v>2.3771023764302599E-2</v>
       </c>
       <c r="G38">
-        <v>0.23035349200504099</v>
+        <v>0.36095558608898498</v>
       </c>
       <c r="H38">
-        <v>5.30627312789166E-2</v>
+        <v>0.13028893512884199</v>
       </c>
       <c r="I38">
         <v>18000</v>
@@ -4858,28 +4858,28 @@
     </row>
     <row r="39" spans="1:9">
       <c r="A39">
-        <v>0.22353836590863699</v>
+        <v>0.156245212770111</v>
       </c>
       <c r="B39">
-        <v>4.9969401033103697E-2</v>
+        <v>2.4412566513577399E-2</v>
       </c>
       <c r="C39">
-        <v>0.21552591211981001</v>
+        <v>0.173727440032865</v>
       </c>
       <c r="D39">
-        <v>4.6451418795076402E-2</v>
+        <v>3.01812234203729E-2</v>
       </c>
       <c r="E39">
-        <v>0.17839437499999999</v>
+        <v>0.15412523467815301</v>
       </c>
       <c r="F39">
-        <v>3.1824552999999998E-2</v>
+        <v>2.37545879645959E-2</v>
       </c>
       <c r="G39">
-        <v>0.23033132311012999</v>
+        <v>0.360903389842191</v>
       </c>
       <c r="H39">
-        <v>5.3052518405663503E-2</v>
+        <v>0.13025125679958399</v>
       </c>
       <c r="I39">
         <v>18500</v>
@@ -4887,28 +4887,28 @@
     </row>
     <row r="40" spans="1:9">
       <c r="A40">
-        <v>0.22316759097231001</v>
+        <v>0.15623805237955099</v>
       </c>
       <c r="B40">
-        <v>4.98037736603845E-2</v>
+        <v>2.4410329011355501E-2</v>
       </c>
       <c r="C40">
-        <v>0.21525335826965</v>
+        <v>0.173743404224598</v>
       </c>
       <c r="D40">
-        <v>4.6334008246362697E-2</v>
+        <v>3.0186770511552299E-2</v>
       </c>
       <c r="E40">
-        <v>0.17843788899999999</v>
+        <v>0.154116126510043</v>
       </c>
       <c r="F40">
-        <v>3.184008E-2</v>
+        <v>2.3751780450459802E-2</v>
       </c>
       <c r="G40">
-        <v>0.22985427644537901</v>
+        <v>0.36085336015939801</v>
       </c>
       <c r="H40">
-        <v>5.2832988400228799E-2</v>
+        <v>0.130215147538328</v>
       </c>
       <c r="I40">
         <v>19000</v>
@@ -4916,28 +4916,28 @@
     </row>
     <row r="41" spans="1:9">
       <c r="A41">
-        <v>0.22280122910560299</v>
+        <v>0.156231751456642</v>
       </c>
       <c r="B41">
-        <v>4.9640387690967298E-2</v>
+        <v>2.4408360163210002E-2</v>
       </c>
       <c r="C41">
-        <v>0.214999639190987</v>
+        <v>0.17376115250617799</v>
       </c>
       <c r="D41">
-        <v>4.6224844852254698E-2</v>
+        <v>3.0192938120275299E-2</v>
       </c>
       <c r="E41">
-        <v>0.17847953999999999</v>
+        <v>0.15416863212078599</v>
       </c>
       <c r="F41">
-        <v>3.1854946000000002E-2</v>
+        <v>2.37679671299942E-2</v>
       </c>
       <c r="G41">
-        <v>0.23057320724352101</v>
+        <v>0.36080536196749002</v>
       </c>
       <c r="H41">
-        <v>5.3164003898563697E-2</v>
+        <v>0.13018050922449101</v>
       </c>
       <c r="I41">
         <v>19500</v>
@@ -4945,28 +4945,28 @@
     </row>
     <row r="42" spans="1:9">
       <c r="A42">
-        <v>0.222439159245096</v>
+        <v>0.156226163915857</v>
       </c>
       <c r="B42">
-        <v>4.9479179565665297E-2</v>
+        <v>2.4406614291864401E-2</v>
       </c>
       <c r="C42">
-        <v>0.21476368561217099</v>
+        <v>0.173780649473433</v>
       </c>
       <c r="D42">
-        <v>4.6123440657723599E-2</v>
+        <v>3.0199714131408199E-2</v>
       </c>
       <c r="E42">
-        <v>0.17851909499999999</v>
+        <v>0.154271742278836</v>
       </c>
       <c r="F42">
-        <v>3.1869067000000001E-2</v>
+        <v>2.3799770465747799E-2</v>
       </c>
       <c r="G42">
-        <v>0.229939824855008</v>
+        <v>0.36075927148181097</v>
       </c>
       <c r="H42">
-        <v>5.2872323054352098E-2</v>
+        <v>0.130147251960087</v>
       </c>
       <c r="I42">
         <v>20000</v>
@@ -4974,28 +4974,28 @@
     </row>
     <row r="43" spans="1:9">
       <c r="A43">
-        <v>0.22208137684463</v>
+        <v>0.15622117172370401</v>
       </c>
       <c r="B43">
-        <v>4.9320137941206897E-2</v>
+        <v>2.4405054494727199E-2</v>
       </c>
       <c r="C43">
-        <v>0.214544479918095</v>
+        <v>0.17380187448325199</v>
       </c>
       <c r="D43">
-        <v>4.6029333863326097E-2</v>
+        <v>3.0207091573892099E-2</v>
       </c>
       <c r="E43">
-        <v>0.17855633000000001</v>
+        <v>0.15439510051163</v>
       </c>
       <c r="F43">
-        <v>3.1882362999999997E-2</v>
+        <v>2.3837847061996299E-2</v>
       </c>
       <c r="G43">
-        <v>0.22970992532408299</v>
+        <v>0.36071497501678401</v>
       </c>
       <c r="H43">
-        <v>5.2766649792396099E-2</v>
+        <v>0.13011529320135901</v>
       </c>
       <c r="I43">
         <v>20500</v>
@@ -5003,28 +5003,28 @@
     </row>
     <row r="44" spans="1:9">
       <c r="A44">
-        <v>0.221727975619123</v>
+        <v>0.15621667901030001</v>
       </c>
       <c r="B44">
-        <v>4.9163295172154502E-2</v>
+        <v>2.44036508010071E-2</v>
       </c>
       <c r="C44">
-        <v>0.214341054666355</v>
+        <v>0.17382482108796199</v>
       </c>
       <c r="D44">
-        <v>4.5942087715485497E-2</v>
+        <v>3.0215068426261999E-2</v>
       </c>
       <c r="E44">
-        <v>0.17859103100000001</v>
+        <v>0.154513454377253</v>
       </c>
       <c r="F44">
-        <v>3.1894756000000003E-2</v>
+        <v>2.3874407583591599E-2</v>
       </c>
       <c r="G44">
-        <v>0.229916436640838</v>
+        <v>0.36067236794776403</v>
       </c>
       <c r="H44">
-        <v>5.2861567837620499E-2</v>
+        <v>0.13008455700104701</v>
       </c>
       <c r="I44">
         <v>21000</v>
@@ -5032,28 +5032,28 @@
     </row>
     <row r="45" spans="1:9">
       <c r="A45">
-        <v>0.22137912588515099</v>
+        <v>0.15621260759963801</v>
       </c>
       <c r="B45">
-        <v>4.9008717377673698E-2</v>
+        <v>2.4402378773078499E-2</v>
       </c>
       <c r="C45">
-        <v>0.21415249040950299</v>
+        <v>0.173849496711556</v>
       </c>
       <c r="D45">
-        <v>4.5861289148592499E-2</v>
+        <v>3.0223647506861399E-2</v>
       </c>
       <c r="E45">
-        <v>0.17862298099999999</v>
+        <v>0.15461369716678899</v>
       </c>
       <c r="F45">
-        <v>3.1906168999999998E-2</v>
+        <v>2.3905395351583598E-2</v>
       </c>
       <c r="G45">
-        <v>0.23005166681847899</v>
+        <v>0.360631353801669</v>
       </c>
       <c r="H45">
-        <v>5.2923769405960601E-2</v>
+        <v>0.13005497334482499</v>
       </c>
       <c r="I45">
         <v>21500</v>
@@ -5061,28 +5061,28 @@
     </row>
     <row r="46" spans="1:9">
       <c r="A46">
-        <v>0.22103505117133701</v>
+        <v>0.15620889354536499</v>
       </c>
       <c r="B46">
-        <v>4.8856493846315699E-2</v>
+        <v>2.44012184226674E-2</v>
       </c>
       <c r="C46">
-        <v>0.21397791245086001</v>
+        <v>0.173875922572961</v>
       </c>
       <c r="D46">
-        <v>4.5786547016828001E-2</v>
+        <v>3.0232836450598599E-2</v>
       </c>
       <c r="E46">
-        <v>0.178651964</v>
+        <v>0.154692036875237</v>
       </c>
       <c r="F46">
-        <v>3.1916524000000002E-2</v>
+        <v>2.3929626272609798E-2</v>
       </c>
       <c r="G46">
-        <v>0.23027196742674699</v>
+        <v>0.36059184345773398</v>
       </c>
       <c r="H46">
-        <v>5.3025178982584902E-2</v>
+        <v>0.13002647756824601</v>
       </c>
       <c r="I46">
         <v>22000</v>
@@ -5090,28 +5090,28 @@
     </row>
     <row r="47" spans="1:9">
       <c r="A47">
-        <v>0.220696004801821</v>
+        <v>0.156205484405677</v>
       </c>
       <c r="B47">
-        <v>4.8706726535485398E-2</v>
+        <v>2.44001533584122E-2</v>
       </c>
       <c r="C47">
-        <v>0.21381648574034501</v>
+        <v>0.17390413387155701</v>
       </c>
       <c r="D47">
-        <v>4.5717489574351101E-2</v>
+        <v>3.0242647777616601E-2</v>
       </c>
       <c r="E47">
-        <v>0.17867775699999999</v>
+        <v>0.15474919154085201</v>
       </c>
       <c r="F47">
-        <v>3.1925741000000001E-2</v>
+        <v>2.3947312282547501E-2</v>
       </c>
       <c r="G47">
-        <v>0.23080871363164401</v>
+        <v>0.36055375444277898</v>
       </c>
       <c r="H47">
-        <v>5.3272662288294401E-2</v>
+        <v>0.12999900984278401</v>
       </c>
       <c r="I47">
         <v>22500</v>
@@ -5119,28 +5119,28 @@
     </row>
     <row r="48" spans="1:9">
       <c r="A48">
-        <v>0.22036224805304599</v>
+        <v>0.15620233707632</v>
       </c>
       <c r="B48">
-        <v>4.8559520366992202E-2</v>
+        <v>2.4399170108104402E-2</v>
       </c>
       <c r="C48">
-        <v>0.213667406227566</v>
+        <v>0.17393418026091201</v>
       </c>
       <c r="D48">
-        <v>4.5653760484015697E-2</v>
+        <v>3.02530990630356E-2</v>
       </c>
       <c r="E48">
-        <v>0.17870012299999999</v>
+        <v>0.15478727228059</v>
       </c>
       <c r="F48">
-        <v>3.1933733999999998E-2</v>
+        <v>2.39590996600656E-2</v>
       </c>
       <c r="G48">
-        <v>0.23162957197523701</v>
+        <v>0.36051701030796901</v>
       </c>
       <c r="H48">
-        <v>5.3652258613431703E-2</v>
+        <v>0.12997251472139601</v>
       </c>
       <c r="I48">
         <v>23000</v>
@@ -5148,28 +5148,28 @@
     </row>
     <row r="49" spans="1:9">
       <c r="A49">
-        <v>0.22003403121857501</v>
+        <v>0.15619941605349599</v>
       </c>
       <c r="B49">
-        <v>4.8414974894297101E-2</v>
+        <v>2.4398257575453199E-2</v>
       </c>
       <c r="C49">
-        <v>0.21352988514611701</v>
+        <v>0.17396612664886901</v>
       </c>
       <c r="D49">
-        <v>4.5595011850513997E-2</v>
+        <v>3.0264213221210302E-2</v>
       </c>
       <c r="E49">
-        <v>0.178718814</v>
+        <v>0.154808503033178</v>
       </c>
       <c r="F49">
-        <v>3.1940415E-2</v>
+        <v>2.3965672611373601E-2</v>
       </c>
       <c r="G49">
-        <v>0.23240248647239001</v>
+        <v>0.36048154007600902</v>
       </c>
       <c r="H49">
-        <v>5.40109157185494E-2</v>
+        <v>0.129946940735571</v>
       </c>
       <c r="I49">
         <v>23500</v>
@@ -5177,28 +5177,28 @@
     </row>
     <row r="50" spans="1:9">
       <c r="A50">
-        <v>0.219711578509827</v>
+        <v>0.15619669203285599</v>
       </c>
       <c r="B50">
-        <v>4.8273177731279898E-2</v>
+        <v>2.4397406602007E-2</v>
       </c>
       <c r="C50">
-        <v>0.21340311894393599</v>
+        <v>0.17400005437628499</v>
       </c>
       <c r="D50">
-        <v>4.5540891174999702E-2</v>
+        <v>3.02760189229501E-2</v>
       </c>
       <c r="E50">
-        <v>0.17873356100000001</v>
+        <v>0.15481486852284601</v>
       </c>
       <c r="F50">
-        <v>3.1945686000000001E-2</v>
+        <v>2.39676435157462E-2</v>
       </c>
       <c r="G50">
-        <v>0.232699948855421</v>
+        <v>0.36044727774951302</v>
       </c>
       <c r="H50">
-        <v>5.4149266197315797E-2</v>
+        <v>0.12992224003703401</v>
       </c>
       <c r="I50">
         <v>24000</v>
@@ -5206,28 +5206,28 @@
     </row>
     <row r="51" spans="1:9">
       <c r="A51">
-        <v>0.219395077237724</v>
+        <v>0.15619414077431701</v>
       </c>
       <c r="B51">
-        <v>4.8134199916147299E-2</v>
+        <v>2.4396609612227199E-2</v>
       </c>
       <c r="C51">
-        <v>0.213286229888627</v>
+        <v>0.17403606284405701</v>
       </c>
       <c r="D51">
-        <v>4.5491015860104497E-2</v>
+        <v>3.0288551170260601E-2</v>
       </c>
       <c r="E51">
-        <v>0.17874407</v>
+        <v>0.15480805657257499</v>
       </c>
       <c r="F51">
-        <v>3.1949442000000002E-2</v>
+        <v>2.3965534379777699E-2</v>
       </c>
       <c r="G51">
-        <v>0.23180669526630199</v>
+        <v>0.360414161872603</v>
       </c>
       <c r="H51">
-        <v>5.3734343970284301E-2</v>
+        <v>0.12989836807833099</v>
       </c>
       <c r="I51">
         <v>24500</v>
@@ -5235,28 +5235,28 @@
     </row>
     <row r="52" spans="1:9">
       <c r="A52">
-        <v>0.219084671247326</v>
+        <v>0.15619174217899201</v>
       </c>
       <c r="B52">
-        <v>4.7998093175548998E-2</v>
+        <v>2.4395860324908699E-2</v>
       </c>
       <c r="C52">
-        <v>0.213178146019807</v>
+        <v>0.174074271679443</v>
       </c>
       <c r="D52">
-        <v>4.5444921940442203E-2</v>
+        <v>3.03018520607287E-2</v>
       </c>
       <c r="E52">
-        <v>0.17875002000000001</v>
+        <v>0.15478946859765899</v>
       </c>
       <c r="F52">
-        <v>3.1951569999999999E-2</v>
+        <v>2.3959779588745699E-2</v>
       </c>
       <c r="G52">
-        <v>0.231879423844041</v>
+        <v>0.36038213513902301</v>
       </c>
       <c r="H52">
-        <v>5.3768067202244599E-2</v>
+        <v>0.12987528332736101</v>
       </c>
       <c r="I52">
         <v>25000</v>
@@ -5264,28 +5264,28 @@
     </row>
     <row r="53" spans="1:9">
       <c r="A53">
-        <v>0.21878045818955699</v>
+        <v>0.15618947953661</v>
       </c>
       <c r="B53">
-        <v>4.7864888885632499E-2</v>
+        <v>2.4395153517917299E-2</v>
       </c>
       <c r="C53">
-        <v>0.21307734852042301</v>
+        <v>0.174114823559784</v>
       </c>
       <c r="D53">
-        <v>4.54019564524938E-2</v>
+        <v>3.0315971783254701E-2</v>
       </c>
       <c r="E53">
-        <v>0.17875105899999999</v>
+        <v>0.15476029037365499</v>
       </c>
       <c r="F53">
-        <v>3.1951940999999998E-2</v>
+        <v>2.3950747476538199E-2</v>
       </c>
       <c r="G53">
-        <v>0.231928405813462</v>
+        <v>0.360351144040986</v>
       </c>
       <c r="H53">
-        <v>5.3790785423174302E-2</v>
+        <v>0.12985294701164701</v>
       </c>
       <c r="I53">
         <v>25500</v>
@@ -5293,28 +5293,28 @@
     </row>
     <row r="54" spans="1:9">
       <c r="A54">
-        <v>0.21848248995709599</v>
+        <v>0.15618733891075301</v>
       </c>
       <c r="B54">
-        <v>4.7734598417852901E-2</v>
+        <v>2.4394484836022402E-2</v>
       </c>
       <c r="C54">
-        <v>0.212981221401285</v>
+        <v>0.174157887846317</v>
       </c>
       <c r="D54">
-        <v>4.53610006695832E-2</v>
+        <v>3.0330969899090399E-2</v>
       </c>
       <c r="E54">
-        <v>0.17874679500000001</v>
+        <v>0.154721691492993</v>
       </c>
       <c r="F54">
-        <v>3.1950417000000002E-2</v>
+        <v>2.3938801818452898E-2</v>
       </c>
       <c r="G54">
-        <v>0.23158021781723001</v>
+        <v>0.36032113855381998</v>
       </c>
       <c r="H54">
-        <v>5.3629397284275702E-2</v>
+        <v>0.12983132288872101</v>
       </c>
       <c r="I54">
         <v>26000</v>
@@ -5322,28 +5322,28 @@
     </row>
     <row r="55" spans="1:9">
       <c r="A55">
-        <v>0.21819077549411001</v>
+        <v>0.156185308635994</v>
       </c>
       <c r="B55">
-        <v>4.7607214510721203E-2</v>
+        <v>2.43938506337209E-2</v>
       </c>
       <c r="C55">
-        <v>0.21288226019697701</v>
+        <v>0.17420366522542499</v>
       </c>
       <c r="D55">
-        <v>4.5318856706573499E-2</v>
+        <v>3.0346916977972201E-2</v>
       </c>
       <c r="E55">
-        <v>0.178736793</v>
+        <v>0.15467520509187899</v>
       </c>
       <c r="F55">
-        <v>3.1946840999999997E-2</v>
+        <v>2.3924419070214999E-2</v>
       </c>
       <c r="G55">
-        <v>0.23135429060547</v>
+        <v>0.36029207185213402</v>
       </c>
       <c r="H55">
-        <v>5.3524807781560498E-2</v>
+        <v>0.12981037703950299</v>
       </c>
       <c r="I55">
         <v>26500</v>
@@ -5351,28 +5351,28 @@
     </row>
     <row r="56" spans="1:9">
       <c r="A56">
-        <v>0.217905285192209</v>
+        <v>0.156183378906252</v>
       </c>
       <c r="B56">
-        <v>4.7482713314698097E-2</v>
+        <v>2.4393247846574002E-2</v>
       </c>
       <c r="C56">
-        <v>0.21269442564528601</v>
+        <v>0.17425239361233499</v>
       </c>
       <c r="D56">
-        <v>4.5238918700578397E-2</v>
+        <v>3.03638966796284E-2</v>
       </c>
       <c r="E56">
-        <v>0.17872057199999999</v>
+        <v>0.15462320084520301</v>
       </c>
       <c r="F56">
-        <v>3.1941043000000002E-2</v>
+        <v>2.3908334239616101E-2</v>
       </c>
       <c r="G56">
-        <v>0.23088357901085699</v>
+        <v>0.36026390005383102</v>
       </c>
       <c r="H56">
-        <v>5.3307227056862701E-2</v>
+        <v>0.12979007768199699</v>
       </c>
       <c r="I56">
         <v>27000</v>
@@ -5380,28 +5380,28 @@
     </row>
     <row r="57" spans="1:9">
       <c r="A57">
-        <v>0.217625956172457</v>
+        <v>0.156181541437664</v>
       </c>
       <c r="B57">
-        <v>4.7361056799976299E-2</v>
+        <v>2.4392673885844901E-2</v>
       </c>
       <c r="C57">
-        <v>0.21328702619741199</v>
+        <v>0.17430435564705499</v>
       </c>
       <c r="D57">
-        <v>4.5491355544135699E-2</v>
+        <v>3.0382008397535201E-2</v>
       </c>
       <c r="E57">
-        <v>0.17869759599999999</v>
+        <v>0.154569087821357</v>
       </c>
       <c r="F57">
-        <v>3.1932831000000002E-2</v>
+        <v>2.3891602909926399E-2</v>
       </c>
       <c r="G57">
-        <v>0.23023554562096199</v>
+        <v>0.36023658198877501</v>
       </c>
       <c r="H57">
-        <v>5.3008406467382398E-2</v>
+        <v>0.12977039500295501</v>
       </c>
       <c r="I57">
         <v>27500</v>
@@ -5409,28 +5409,28 @@
     </row>
     <row r="58" spans="1:9">
       <c r="A58">
-        <v>0.217352697886569</v>
+        <v>0.15617978919249201</v>
       </c>
       <c r="B58">
-        <v>4.7242195278570397E-2</v>
+        <v>2.4392126552211301E-2</v>
       </c>
       <c r="C58">
-        <v>0.213579440333556</v>
+        <v>0.17435988820855</v>
       </c>
       <c r="D58">
-        <v>4.5616177333195299E-2</v>
+        <v>3.0401370616098301E-2</v>
       </c>
       <c r="E58">
-        <v>0.17866727199999999</v>
+        <v>0.15451675732677</v>
       </c>
       <c r="F58">
-        <v>3.1921994000000002E-2</v>
+        <v>2.387542829478E-2</v>
       </c>
       <c r="G58">
-        <v>0.23021748772703701</v>
+        <v>0.36021007898933199</v>
       </c>
       <c r="H58">
-        <v>5.30000916553484E-2</v>
+        <v>0.129751301005501</v>
       </c>
       <c r="I58">
         <v>28000</v>
@@ -5438,28 +5438,28 @@
     </row>
     <row r="59" spans="1:9">
       <c r="A59">
-        <v>0.21708539761772799</v>
+        <v>0.15617811615307001</v>
       </c>
       <c r="B59">
-        <v>4.7126069858847097E-2</v>
+        <v>2.43916039651219E-2</v>
       </c>
       <c r="C59">
-        <v>0.21527029717107099</v>
+        <v>0.17441939449583799</v>
       </c>
       <c r="D59">
-        <v>4.6341300844121497E-2</v>
+        <v>3.0422125176295001E-2</v>
       </c>
       <c r="E59">
-        <v>0.17862893899999999</v>
+        <v>0.15446949415959499</v>
       </c>
       <c r="F59">
-        <v>3.1908298000000002E-2</v>
+        <v>2.3860824625921099E-2</v>
       </c>
       <c r="G59">
-        <v>0.229965288926331</v>
+        <v>0.36018435470037802</v>
       </c>
       <c r="H59">
-        <v>5.2884034110971097E-2</v>
+        <v>0.12973276937092801</v>
       </c>
       <c r="I59">
         <v>28500</v>
@@ -5467,28 +5467,28 @@
     </row>
     <row r="60" spans="1:9">
       <c r="A60">
-        <v>0.21682392559958499</v>
+        <v>0.15617651713683101</v>
       </c>
       <c r="B60">
-        <v>4.7012614712414601E-2</v>
+        <v>2.43911045049909E-2</v>
       </c>
       <c r="C60">
-        <v>0.21750376820204501</v>
+        <v>0.17448335937756701</v>
       </c>
       <c r="D60">
-        <v>4.7307889182088898E-2</v>
+        <v>3.0444442699681201E-2</v>
       </c>
       <c r="E60">
-        <v>0.178581872</v>
+        <v>0.15442983965768101</v>
       </c>
       <c r="F60">
-        <v>3.1891484999999997E-2</v>
+        <v>2.3848575376697101E-2</v>
       </c>
       <c r="G60">
-        <v>0.230114476755613</v>
+        <v>0.36015937490665301</v>
       </c>
       <c r="H60">
-        <v>5.2952672412509602E-2</v>
+        <v>0.12971477533315101</v>
       </c>
       <c r="I60">
         <v>29000</v>
@@ -5496,28 +5496,28 @@
     </row>
     <row r="61" spans="1:9">
       <c r="A61">
-        <v>0.216568139588484</v>
+        <v>0.156174987645053</v>
       </c>
       <c r="B61">
-        <v>4.6901759084817203E-2</v>
+        <v>2.4390626765932601E-2</v>
       </c>
       <c r="C61">
-        <v>0.223132794684201</v>
+        <v>0.17455236889482401</v>
       </c>
       <c r="D61">
-        <v>4.97882440635821E-2</v>
+        <v>3.0468529486794699E-2</v>
       </c>
       <c r="E61">
-        <v>0.17852527000000001</v>
+        <v>0.154401282859224</v>
       </c>
       <c r="F61">
-        <v>3.1871271999999999E-2</v>
+        <v>2.3839756148574101E-2</v>
       </c>
       <c r="G61">
-        <v>0.230089540773493</v>
+        <v>0.360135107375603</v>
       </c>
       <c r="H61">
-        <v>5.2941196773357103E-2</v>
+        <v>0.12969729556443699</v>
       </c>
       <c r="I61">
         <v>29500</v>
@@ -5525,37 +5525,37 @@
     </row>
     <row r="62" spans="1:9">
       <c r="A62">
-        <v>0.216317888814062</v>
+        <v>0.15617352373930701</v>
       </c>
       <c r="B62">
-        <v>4.6793429020972901E-2</v>
+        <v>2.4390169517152099E-2</v>
       </c>
       <c r="C62">
-        <v>0.23498739864527499</v>
+        <v>0.17462713500482599</v>
       </c>
       <c r="D62">
-        <v>5.5219077522073702E-2</v>
+        <v>3.04946362799937E-2</v>
       </c>
       <c r="E62">
-        <v>0.17845825500000001</v>
+        <v>0.154390133809026</v>
       </c>
       <c r="F62">
-        <v>3.1847348999999997E-2</v>
+        <v>2.3836313417569199E-2</v>
       </c>
       <c r="G62">
-        <v>0.22953008495330701</v>
+        <v>0.36011152171411898</v>
       </c>
       <c r="H62">
-        <v>5.2684059898672399E-2</v>
+        <v>0.12968030807125799</v>
       </c>
       <c r="I62">
         <v>30000</v>
       </c>
     </row>
   </sheetData>
+  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <drawing r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">

</xml_diff>

<commit_message>
Neural Network updates. Removal of unnessary code
</commit_message>
<xml_diff>
--- a/Year3_Project/Documents/Evaluations/Weekly Comparison.xlsx
+++ b/Year3_Project/Documents/Evaluations/Weekly Comparison.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>6-3 RMSE</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -54,6 +54,10 @@
   </si>
   <si>
     <t>Number of Epochs</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -112,15 +116,15 @@
       <c:lineChart>
         <c:grouping val="standard"/>
         <c:ser>
-          <c:idx val="3"/>
+          <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$1</c:f>
+              <c:f>Sheet1!$B$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>6-3 RMSE</c:v>
+                  <c:v>6-3 MSE</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -324,207 +328,207 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$62</c:f>
+              <c:f>Sheet1!$B$2:$B$62</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="61"/>
                 <c:pt idx="0">
-                  <c:v>0.170891063275283</c:v>
+                  <c:v>0.0292037555073571</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.176734624494346</c:v>
+                  <c:v>0.0312351274951576</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.189655529393182</c:v>
+                  <c:v>0.0359692198294083</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.190269088468723</c:v>
+                  <c:v>0.0362023260267188</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.18579585650666</c:v>
+                  <c:v>0.0345201002950436</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.182765517322699</c:v>
+                  <c:v>0.033403234322234</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.179319716808685</c:v>
+                  <c:v>0.0321555608363472</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.174464241845423</c:v>
+                  <c:v>0.0304377716826984</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.170802133462548</c:v>
+                  <c:v>0.0291733687953581</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.168570445993694</c:v>
+                  <c:v>0.0284159952625131</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.167612878029524</c:v>
+                  <c:v>0.0280940768813403</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.167095237103902</c:v>
+                  <c:v>0.0279208182628094</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.1668394964107</c:v>
+                  <c:v>0.0278354175625761</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.166666772436607</c:v>
+                  <c:v>0.0277778130344359</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.166514514398946</c:v>
+                  <c:v>0.0277270835055169</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.16636592861863</c:v>
+                  <c:v>0.0276776222051391</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.166200331154002</c:v>
+                  <c:v>0.0276225500757001</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.165975014412715</c:v>
+                  <c:v>0.027547705409301</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.165597329195588</c:v>
+                  <c:v>0.0274224754367121</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.164875003659872</c:v>
+                  <c:v>0.0271837668318429</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0.163513597041372</c:v>
+                  <c:v>0.0267366964174081</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>0.161432625392691</c:v>
+                  <c:v>0.0260604925411769</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>0.159283552632882</c:v>
+                  <c:v>0.0253712501393523</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>0.157832845861242</c:v>
+                  <c:v>0.0249112072326587</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>0.157088083235906</c:v>
+                  <c:v>0.0246766658947311</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>0.156736964206873</c:v>
+                  <c:v>0.0245664759487868</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>0.156564748772609</c:v>
+                  <c:v>0.0245125205582302</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>0.15647099879605</c:v>
+                  <c:v>0.0244831734642337</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>0.156413260150052</c:v>
+                  <c:v>0.0244651079507679</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>0.156373615807565</c:v>
+                  <c:v>0.0244527077207322</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>0.156344144680854</c:v>
+                  <c:v>0.024443491575988</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>0.156321062487683</c:v>
+                  <c:v>0.0244362745772782</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>0.156302374631209</c:v>
+                  <c:v>0.024430432315355</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>0.156286913269957</c:v>
+                  <c:v>0.024425599259451</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>0.156273925610435</c:v>
+                  <c:v>0.0244215398256958</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>0.156262887800976</c:v>
+                  <c:v>0.0244180901039004</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>0.156253414755249</c:v>
+                  <c:v>0.024415129622676</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>0.156245212770111</c:v>
+                  <c:v>0.0244125665135774</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>0.156238052379551</c:v>
+                  <c:v>0.0244103290113555</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>0.156231751456642</c:v>
+                  <c:v>0.02440836016321</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>0.156226163915857</c:v>
+                  <c:v>0.0244066142918644</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>0.156221171723704</c:v>
+                  <c:v>0.0244050544947272</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>0.1562166790103</c:v>
+                  <c:v>0.0244036508010071</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>0.156212607599638</c:v>
+                  <c:v>0.0244023787730785</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>0.156208893545365</c:v>
+                  <c:v>0.0244012184226674</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>0.156205484405677</c:v>
+                  <c:v>0.0244001533584122</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>0.15620233707632</c:v>
+                  <c:v>0.0243991701081044</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>0.156199416053496</c:v>
+                  <c:v>0.0243982575754532</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>0.156196692032856</c:v>
+                  <c:v>0.024397406602007</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>0.156194140774317</c:v>
+                  <c:v>0.0243966096122272</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>0.156191742178992</c:v>
+                  <c:v>0.0243958603249087</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>0.15618947953661</c:v>
+                  <c:v>0.0243951535179173</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>0.156187338910753</c:v>
+                  <c:v>0.0243944848360224</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>0.156185308635994</c:v>
+                  <c:v>0.0243938506337209</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>0.156183378906252</c:v>
+                  <c:v>0.024393247846574</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>0.156181541437664</c:v>
+                  <c:v>0.0243926738858449</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>0.156179789192492</c:v>
+                  <c:v>0.0243921265522113</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>0.15617811615307</c:v>
+                  <c:v>0.0243916039651219</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>0.156176517136831</c:v>
+                  <c:v>0.0243911045049909</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>0.156174987645053</c:v>
+                  <c:v>0.0243906267659326</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>0.156173523739307</c:v>
+                  <c:v>0.0243901695171521</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
         <c:ser>
-          <c:idx val="0"/>
+          <c:idx val="2"/>
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$B$1</c:f>
+              <c:f>Sheet1!$D$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>6-3 MSE</c:v>
+                  <c:v>6-4 MSE</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -728,207 +732,207 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$B$62</c:f>
+              <c:f>Sheet1!$D$2:$D$62</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="61"/>
                 <c:pt idx="0">
-                  <c:v>0.0292037555073571</c:v>
+                  <c:v>0.0617950181467108</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.0312351274951576</c:v>
+                  <c:v>0.0350726944985074</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.0359692198294083</c:v>
+                  <c:v>0.033444334806742</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.0362023260267188</c:v>
+                  <c:v>0.0325952494446254</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.0345201002950436</c:v>
+                  <c:v>0.0320382148297012</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.033403234322234</c:v>
+                  <c:v>0.0316398123040048</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.0321555608363472</c:v>
+                  <c:v>0.0313427175772398</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.0304377716826984</c:v>
+                  <c:v>0.0311155319863906</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.0291733687953581</c:v>
+                  <c:v>0.0309385899682655</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.0284159952625131</c:v>
+                  <c:v>0.0307986622673226</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.0280940768813403</c:v>
+                  <c:v>0.0306865088342104</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.0279208182628094</c:v>
+                  <c:v>0.0305955356665266</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.0278354175625761</c:v>
+                  <c:v>0.0305209649365542</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.0277778130344359</c:v>
+                  <c:v>0.0304592880255975</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.0277270835055169</c:v>
+                  <c:v>0.0304078940372854</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.0276776222051391</c:v>
+                  <c:v>0.0303648139073907</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.0276225500757001</c:v>
+                  <c:v>0.0303285425681121</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.027547705409301</c:v>
+                  <c:v>0.0302979143401367</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.0274224754367121</c:v>
+                  <c:v>0.0302720148336606</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.0271837668318429</c:v>
+                  <c:v>0.0302501180403276</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0.0267366964174081</c:v>
+                  <c:v>0.0302316409335622</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>0.0260604925411769</c:v>
+                  <c:v>0.030216110342876</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>0.0253712501393523</c:v>
+                  <c:v>0.0302031385155863</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>0.0249112072326587</c:v>
+                  <c:v>0.0301924048903905</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>0.0246766658947311</c:v>
+                  <c:v>0.0301836423593551</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>0.0245664759487868</c:v>
+                  <c:v>0.0301766268071519</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>0.0245125205582302</c:v>
+                  <c:v>0.0301711690679597</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>0.0244831734642337</c:v>
+                  <c:v>0.0301671086838499</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>0.0244651079507679</c:v>
+                  <c:v>0.0301643090185532</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>0.0244527077207322</c:v>
+                  <c:v>0.0301626534005118</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>0.024443491575988</c:v>
+                  <c:v>0.0301620420546331</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>0.0244362745772782</c:v>
+                  <c:v>0.0301623896437177</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>0.024430432315355</c:v>
+                  <c:v>0.0301636232852793</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>0.024425599259451</c:v>
+                  <c:v>0.0301656809423586</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>0.0244215398256958</c:v>
+                  <c:v>0.0301685101113126</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>0.0244180901039004</c:v>
+                  <c:v>0.0301720667478846</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>0.024415129622676</c:v>
+                  <c:v>0.0301763143867427</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>0.0244125665135774</c:v>
+                  <c:v>0.0301812234203729</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>0.0244103290113555</c:v>
+                  <c:v>0.0301867705115523</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>0.02440836016321</c:v>
+                  <c:v>0.0301929381202753</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>0.0244066142918644</c:v>
+                  <c:v>0.0301997141314082</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>0.0244050544947272</c:v>
+                  <c:v>0.0302070915738921</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>0.0244036508010071</c:v>
+                  <c:v>0.030215068426262</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>0.0244023787730785</c:v>
+                  <c:v>0.0302236475068614</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>0.0244012184226674</c:v>
+                  <c:v>0.0302328364505986</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>0.0244001533584122</c:v>
+                  <c:v>0.0302426477776166</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>0.0243991701081044</c:v>
+                  <c:v>0.0302530990630356</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>0.0243982575754532</c:v>
+                  <c:v>0.0302642132212103</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>0.024397406602007</c:v>
+                  <c:v>0.0302760189229501</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>0.0243966096122272</c:v>
+                  <c:v>0.0302885511702606</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>0.0243958603249087</c:v>
+                  <c:v>0.0303018520607287</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>0.0243951535179173</c:v>
+                  <c:v>0.0303159717832547</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>0.0243944848360224</c:v>
+                  <c:v>0.0303309698990904</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>0.0243938506337209</c:v>
+                  <c:v>0.0303469169779722</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>0.024393247846574</c:v>
+                  <c:v>0.0303638966796284</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>0.0243926738858449</c:v>
+                  <c:v>0.0303820083975352</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>0.0243921265522113</c:v>
+                  <c:v>0.0304013706160983</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>0.0243916039651219</c:v>
+                  <c:v>0.030422125176295</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>0.0243911045049909</c:v>
+                  <c:v>0.0304444426996812</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>0.0243906267659326</c:v>
+                  <c:v>0.0304685294867947</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>0.0243901695171521</c:v>
+                  <c:v>0.0304946362799937</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
         <c:ser>
-          <c:idx val="1"/>
+          <c:idx val="5"/>
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$C$1</c:f>
+              <c:f>Sheet1!$F$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>6-4 RMSE</c:v>
+                  <c:v>6-5 MSE</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1132,207 +1136,207 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$2:$C$62</c:f>
+              <c:f>Sheet1!$F$2:$F$62</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="61"/>
                 <c:pt idx="0">
-                  <c:v>0.248586037714733</c:v>
+                  <c:v>0.0286426094981949</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.187277052781453</c:v>
+                  <c:v>0.0246405232048601</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.182877923234987</c:v>
+                  <c:v>0.0243003578764564</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.180541544926993</c:v>
+                  <c:v>0.0244258065238682</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.178992220025623</c:v>
+                  <c:v>0.0245046637403604</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.177875833951677</c:v>
+                  <c:v>0.0245694021036896</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.17703874597737</c:v>
+                  <c:v>0.024632286864307</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.176395952295937</c:v>
+                  <c:v>0.0246848048965329</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.175893689392955</c:v>
+                  <c:v>0.0247227783312651</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.175495476486781</c:v>
+                  <c:v>0.0247404425621559</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.175175651373729</c:v>
+                  <c:v>0.0247236839295006</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.174915795932004</c:v>
+                  <c:v>0.0246796175064117</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.174702504093542</c:v>
+                  <c:v>0.0246333364331891</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.174525895000133</c:v>
+                  <c:v>0.024578508108104</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.174378593976684</c:v>
+                  <c:v>0.0244859667596949</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.174255025486758</c:v>
+                  <c:v>0.0243674768996683</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.174150918941337</c:v>
+                  <c:v>0.0242512438823396</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.17406296085077</c:v>
+                  <c:v>0.0241042722301126</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.173988547995724</c:v>
+                  <c:v>0.0242632919020453</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.173925610651012</c:v>
+                  <c:v>0.02486259950475</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0.173872484693703</c:v>
+                  <c:v>0.0253103017648577</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>0.17382781809272</c:v>
+                  <c:v>0.025738345967532</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>0.173790501799109</c:v>
+                  <c:v>0.0260006141462633</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>0.173759618123402</c:v>
+                  <c:v>0.0259830090324346</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>0.173734401772807</c:v>
+                  <c:v>0.0254227233918636</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>0.173714210147448</c:v>
+                  <c:v>0.0249760817102182</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>0.173698500477004</c:v>
+                  <c:v>0.024824051847494</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>0.173686812060817</c:v>
+                  <c:v>0.0247099238489416</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>0.173678752352016</c:v>
+                  <c:v>0.0245347500143312</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>0.173673985963677</c:v>
+                  <c:v>0.024331212540569</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>0.173672225916043</c:v>
+                  <c:v>0.0241594931838091</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>0.173673226617454</c:v>
+                  <c:v>0.0240358995096242</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>0.173676778198121</c:v>
+                  <c:v>0.023948114265573</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>0.17368270190885</c:v>
+                  <c:v>0.0238832395269682</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>0.173690846365928</c:v>
+                  <c:v>0.0238342128336998</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>0.173701084475269</c:v>
+                  <c:v>0.0237974742656159</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>0.173713310908354</c:v>
+                  <c:v>0.0237710237643026</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>0.173727440032865</c:v>
+                  <c:v>0.0237545879645959</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>0.173743404224598</c:v>
+                  <c:v>0.0237517804504598</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>0.173761152506178</c:v>
+                  <c:v>0.0237679671299942</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>0.173780649473433</c:v>
+                  <c:v>0.0237997704657478</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>0.173801874483252</c:v>
+                  <c:v>0.0238378470619963</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>0.173824821087962</c:v>
+                  <c:v>0.0238744075835916</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>0.173849496711556</c:v>
+                  <c:v>0.0239053953515836</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>0.173875922572961</c:v>
+                  <c:v>0.0239296262726098</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>0.173904133871557</c:v>
+                  <c:v>0.0239473122825475</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>0.173934180260912</c:v>
+                  <c:v>0.0239590996600656</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>0.173966126648869</c:v>
+                  <c:v>0.0239656726113736</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>0.174000054376285</c:v>
+                  <c:v>0.0239676435157462</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>0.174036062844057</c:v>
+                  <c:v>0.0239655343797777</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>0.174074271679443</c:v>
+                  <c:v>0.0239597795887457</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>0.174114823559784</c:v>
+                  <c:v>0.0239507474765382</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>0.174157887846317</c:v>
+                  <c:v>0.0239388018184529</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>0.174203665225425</c:v>
+                  <c:v>0.023924419070215</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>0.174252393612335</c:v>
+                  <c:v>0.0239083342396161</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>0.174304355647055</c:v>
+                  <c:v>0.0238916029099264</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>0.17435988820855</c:v>
+                  <c:v>0.02387542829478</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>0.174419394495838</c:v>
+                  <c:v>0.0238608246259211</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>0.174483359377567</c:v>
+                  <c:v>0.0238485753766971</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>0.174552368894824</c:v>
+                  <c:v>0.0238397561485741</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>0.174627135004826</c:v>
+                  <c:v>0.0238363134175692</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
         <c:ser>
-          <c:idx val="2"/>
+          <c:idx val="7"/>
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$D$1</c:f>
+              <c:f>Sheet1!$H$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>6-4 MSE</c:v>
+                  <c:v>6-6 MSE</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1536,207 +1540,265 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$D$2:$D$62</c:f>
+              <c:f>Sheet1!$H$2:$H$62</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="61"/>
                 <c:pt idx="0">
-                  <c:v>0.0617950181467108</c:v>
+                  <c:v>0.323952370964491</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.0350726944985074</c:v>
+                  <c:v>0.141892044975742</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.033444334806742</c:v>
+                  <c:v>0.138300520864452</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.0325952494446254</c:v>
+                  <c:v>0.136588939873614</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.0320382148297012</c:v>
+                  <c:v>0.135510033009632</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.0316398123040048</c:v>
+                  <c:v>0.13474564201022</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.0313427175772398</c:v>
+                  <c:v>0.134166165325115</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.0311155319863906</c:v>
+                  <c:v>0.133706870144534</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.0309385899682655</c:v>
+                  <c:v>0.133331025532177</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.0307986622673226</c:v>
+                  <c:v>0.133015920363919</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.0306865088342104</c:v>
+                  <c:v>0.132746635210976</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.0305955356665266</c:v>
+                  <c:v>0.132512917249489</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.0305209649365542</c:v>
+                  <c:v>0.132307466984589</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.0304592880255975</c:v>
+                  <c:v>0.132124934668753</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.0304078940372854</c:v>
+                  <c:v>0.131961302026102</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.0303648139073907</c:v>
+                  <c:v>0.131813485983574</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.0303285425681121</c:v>
+                  <c:v>0.131679076401845</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.0302979143401367</c:v>
+                  <c:v>0.131556157744349</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.0302720148336606</c:v>
+                  <c:v>0.131443184954413</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.0302501180403276</c:v>
+                  <c:v>0.131338895257088</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0.0302316409335622</c:v>
+                  <c:v>0.131242244310431</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>0.030216110342876</c:v>
+                  <c:v>0.131152359194236</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>0.0302031385155863</c:v>
+                  <c:v>0.131068503254373</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>0.0301924048903905</c:v>
+                  <c:v>0.130990049434417</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>0.0301836423593551</c:v>
+                  <c:v>0.130916459776837</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>0.0301766268071519</c:v>
+                  <c:v>0.130847269473027</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>0.0301711690679597</c:v>
+                  <c:v>0.130782074311773</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>0.0301671086838499</c:v>
+                  <c:v>0.13072052069818</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>0.0301643090185532</c:v>
+                  <c:v>0.130662297639266</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>0.0301626534005118</c:v>
+                  <c:v>0.130607130250547</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>0.0301620420546331</c:v>
+                  <c:v>0.130554774450812</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>0.0301623896437177</c:v>
+                  <c:v>0.130505012593877</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>0.0301636232852793</c:v>
+                  <c:v>0.130457649845751</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>0.0301656809423586</c:v>
+                  <c:v>0.130412511159747</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>0.0301685101113126</c:v>
+                  <c:v>0.13036943873494</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>0.0301720667478846</c:v>
+                  <c:v>0.130328289868193</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>0.0301763143867427</c:v>
+                  <c:v>0.130288935128842</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>0.0301812234203729</c:v>
+                  <c:v>0.130251256799584</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>0.0301867705115523</c:v>
+                  <c:v>0.130215147538328</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>0.0301929381202753</c:v>
+                  <c:v>0.130180509224491</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>0.0301997141314082</c:v>
+                  <c:v>0.130147251960087</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>0.0302070915738921</c:v>
+                  <c:v>0.130115293201359</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>0.030215068426262</c:v>
+                  <c:v>0.130084557001047</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>0.0302236475068614</c:v>
+                  <c:v>0.130054973344825</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>0.0302328364505986</c:v>
+                  <c:v>0.130026477568246</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>0.0302426477776166</c:v>
+                  <c:v>0.129999009842784</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>0.0302530990630356</c:v>
+                  <c:v>0.129972514721396</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>0.0302642132212103</c:v>
+                  <c:v>0.129946940735571</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>0.0302760189229501</c:v>
+                  <c:v>0.129922240037034</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>0.0302885511702606</c:v>
+                  <c:v>0.129898368078331</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>0.0303018520607287</c:v>
+                  <c:v>0.129875283327361</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>0.0303159717832547</c:v>
+                  <c:v>0.129852947011647</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>0.0303309698990904</c:v>
+                  <c:v>0.129831322888721</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>0.0303469169779722</c:v>
+                  <c:v>0.129810377039503</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>0.0303638966796284</c:v>
+                  <c:v>0.129790077681997</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>0.0303820083975352</c:v>
+                  <c:v>0.129770395002955</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>0.0304013706160983</c:v>
+                  <c:v>0.129751301005501</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>0.030422125176295</c:v>
+                  <c:v>0.129732769370928</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>0.0304444426996812</c:v>
+                  <c:v>0.129714775333151</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>0.0304685294867947</c:v>
+                  <c:v>0.129697295564437</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>0.0304946362799937</c:v>
+                  <c:v>0.129680308071258</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
+        <c:marker val="1"/>
+        <c:axId val="291698088"/>
+        <c:axId val="292199640"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="291698088"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="292199640"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="292199640"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="291698088"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+        <c:majorUnit val="0.01"/>
+        <c:minorUnit val="0.001"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="1"/>
+  <c:lang val="en-US"/>
+  <c:style val="2"/>
+  <c:chart>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
         <c:ser>
-          <c:idx val="4"/>
-          <c:order val="4"/>
+          <c:idx val="3"/>
+          <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$E$1</c:f>
+              <c:f>Sheet1!$A$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>6-5 RMSE</c:v>
+                  <c:v>6-3 RMSE</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1940,207 +2002,207 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$E$2:$E$62</c:f>
+              <c:f>Sheet1!$A$2:$A$62</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="61"/>
                 <c:pt idx="0">
-                  <c:v>0.169241275988439</c:v>
+                  <c:v>0.170891063275283</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.156973001515738</c:v>
+                  <c:v>0.176734624494346</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.155885720566241</c:v>
+                  <c:v>0.189655529393182</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.156287576358033</c:v>
+                  <c:v>0.190269088468723</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.156539655488187</c:v>
+                  <c:v>0.18579585650666</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.156746298532659</c:v>
+                  <c:v>0.182765517322699</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.156946764427646</c:v>
+                  <c:v>0.179319716808685</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.157113986953844</c:v>
+                  <c:v>0.174464241845423</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.157234787280885</c:v>
+                  <c:v>0.170802133462548</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.157290948761065</c:v>
+                  <c:v>0.168570445993694</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.157237667018754</c:v>
+                  <c:v>0.167612878029524</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.157097477721355</c:v>
+                  <c:v>0.167095237103902</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.156950108101871</c:v>
+                  <c:v>0.1668394964107</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.156775342793769</c:v>
+                  <c:v>0.166666772436607</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.156479924462197</c:v>
+                  <c:v>0.166514514398946</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.156100854897301</c:v>
+                  <c:v>0.16636592861863</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.155728108838255</c:v>
+                  <c:v>0.166200331154002</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.155255506279528</c:v>
+                  <c:v>0.165975014412715</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.155766786902874</c:v>
+                  <c:v>0.165597329195588</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.157678785842452</c:v>
+                  <c:v>0.164875003659872</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0.15909211723042</c:v>
+                  <c:v>0.163513597041372</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>0.160431748627047</c:v>
+                  <c:v>0.161432625392691</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>0.161247059341444</c:v>
+                  <c:v>0.159283552632882</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>0.161192459601665</c:v>
+                  <c:v>0.157832845861242</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>0.159445048188595</c:v>
+                  <c:v>0.157088083235906</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>0.15803822863541</c:v>
+                  <c:v>0.156736964206873</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>0.157556503666126</c:v>
+                  <c:v>0.156564748772609</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>0.157193905253803</c:v>
+                  <c:v>0.15647099879605</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>0.156635723940393</c:v>
+                  <c:v>0.156413260150052</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>0.155984654824021</c:v>
+                  <c:v>0.156373615807565</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>0.155433243496393</c:v>
+                  <c:v>0.156344144680854</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>0.155035155721611</c:v>
+                  <c:v>0.156321062487683</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>0.154751782754102</c:v>
+                  <c:v>0.156302374631209</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>0.154542031586776</c:v>
+                  <c:v>0.156286913269957</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>0.154383330815537</c:v>
+                  <c:v>0.156273925610435</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>0.154264300036061</c:v>
+                  <c:v>0.156262887800976</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>0.154178545084271</c:v>
+                  <c:v>0.156253414755249</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>0.154125234678153</c:v>
+                  <c:v>0.156245212770111</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>0.154116126510043</c:v>
+                  <c:v>0.156238052379551</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>0.154168632120786</c:v>
+                  <c:v>0.156231751456642</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>0.154271742278836</c:v>
+                  <c:v>0.156226163915857</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>0.15439510051163</c:v>
+                  <c:v>0.156221171723704</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>0.154513454377253</c:v>
+                  <c:v>0.1562166790103</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>0.154613697166789</c:v>
+                  <c:v>0.156212607599638</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>0.154692036875237</c:v>
+                  <c:v>0.156208893545365</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>0.154749191540852</c:v>
+                  <c:v>0.156205484405677</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>0.15478727228059</c:v>
+                  <c:v>0.15620233707632</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>0.154808503033178</c:v>
+                  <c:v>0.156199416053496</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>0.154814868522846</c:v>
+                  <c:v>0.156196692032856</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>0.154808056572575</c:v>
+                  <c:v>0.156194140774317</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>0.154789468597659</c:v>
+                  <c:v>0.156191742178992</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>0.154760290373655</c:v>
+                  <c:v>0.15618947953661</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>0.154721691492993</c:v>
+                  <c:v>0.156187338910753</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>0.154675205091879</c:v>
+                  <c:v>0.156185308635994</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>0.154623200845203</c:v>
+                  <c:v>0.156183378906252</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>0.154569087821357</c:v>
+                  <c:v>0.156181541437664</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>0.15451675732677</c:v>
+                  <c:v>0.156179789192492</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>0.154469494159595</c:v>
+                  <c:v>0.15617811615307</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>0.154429839657681</c:v>
+                  <c:v>0.156176517136831</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>0.154401282859224</c:v>
+                  <c:v>0.156174987645053</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>0.154390133809026</c:v>
+                  <c:v>0.156173523739307</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
         <c:ser>
-          <c:idx val="5"/>
-          <c:order val="5"/>
+          <c:idx val="1"/>
+          <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$F$1</c:f>
+              <c:f>Sheet1!$C$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>6-5 MSE</c:v>
+                  <c:v>6-4 RMSE</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2344,207 +2406,207 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$F$2:$F$62</c:f>
+              <c:f>Sheet1!$C$2:$C$62</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="61"/>
                 <c:pt idx="0">
-                  <c:v>0.0286426094981949</c:v>
+                  <c:v>0.248586037714733</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.0246405232048601</c:v>
+                  <c:v>0.187277052781453</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.0243003578764564</c:v>
+                  <c:v>0.182877923234987</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.0244258065238682</c:v>
+                  <c:v>0.180541544926993</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.0245046637403604</c:v>
+                  <c:v>0.178992220025623</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.0245694021036896</c:v>
+                  <c:v>0.177875833951677</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.024632286864307</c:v>
+                  <c:v>0.17703874597737</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.0246848048965329</c:v>
+                  <c:v>0.176395952295937</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.0247227783312651</c:v>
+                  <c:v>0.175893689392955</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.0247404425621559</c:v>
+                  <c:v>0.175495476486781</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.0247236839295006</c:v>
+                  <c:v>0.175175651373729</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.0246796175064117</c:v>
+                  <c:v>0.174915795932004</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.0246333364331891</c:v>
+                  <c:v>0.174702504093542</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.024578508108104</c:v>
+                  <c:v>0.174525895000133</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.0244859667596949</c:v>
+                  <c:v>0.174378593976684</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.0243674768996683</c:v>
+                  <c:v>0.174255025486758</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.0242512438823396</c:v>
+                  <c:v>0.174150918941337</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.0241042722301126</c:v>
+                  <c:v>0.17406296085077</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.0242632919020453</c:v>
+                  <c:v>0.173988547995724</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.02486259950475</c:v>
+                  <c:v>0.173925610651012</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0.0253103017648577</c:v>
+                  <c:v>0.173872484693703</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>0.025738345967532</c:v>
+                  <c:v>0.17382781809272</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>0.0260006141462633</c:v>
+                  <c:v>0.173790501799109</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>0.0259830090324346</c:v>
+                  <c:v>0.173759618123402</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>0.0254227233918636</c:v>
+                  <c:v>0.173734401772807</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>0.0249760817102182</c:v>
+                  <c:v>0.173714210147448</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>0.024824051847494</c:v>
+                  <c:v>0.173698500477004</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>0.0247099238489416</c:v>
+                  <c:v>0.173686812060817</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>0.0245347500143312</c:v>
+                  <c:v>0.173678752352016</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>0.024331212540569</c:v>
+                  <c:v>0.173673985963677</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>0.0241594931838091</c:v>
+                  <c:v>0.173672225916043</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>0.0240358995096242</c:v>
+                  <c:v>0.173673226617454</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>0.023948114265573</c:v>
+                  <c:v>0.173676778198121</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>0.0238832395269682</c:v>
+                  <c:v>0.17368270190885</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>0.0238342128336998</c:v>
+                  <c:v>0.173690846365928</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>0.0237974742656159</c:v>
+                  <c:v>0.173701084475269</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>0.0237710237643026</c:v>
+                  <c:v>0.173713310908354</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>0.0237545879645959</c:v>
+                  <c:v>0.173727440032865</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>0.0237517804504598</c:v>
+                  <c:v>0.173743404224598</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>0.0237679671299942</c:v>
+                  <c:v>0.173761152506178</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>0.0237997704657478</c:v>
+                  <c:v>0.173780649473433</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>0.0238378470619963</c:v>
+                  <c:v>0.173801874483252</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>0.0238744075835916</c:v>
+                  <c:v>0.173824821087962</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>0.0239053953515836</c:v>
+                  <c:v>0.173849496711556</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>0.0239296262726098</c:v>
+                  <c:v>0.173875922572961</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>0.0239473122825475</c:v>
+                  <c:v>0.173904133871557</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>0.0239590996600656</c:v>
+                  <c:v>0.173934180260912</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>0.0239656726113736</c:v>
+                  <c:v>0.173966126648869</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>0.0239676435157462</c:v>
+                  <c:v>0.174000054376285</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>0.0239655343797777</c:v>
+                  <c:v>0.174036062844057</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>0.0239597795887457</c:v>
+                  <c:v>0.174074271679443</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>0.0239507474765382</c:v>
+                  <c:v>0.174114823559784</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>0.0239388018184529</c:v>
+                  <c:v>0.174157887846317</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>0.023924419070215</c:v>
+                  <c:v>0.174203665225425</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>0.0239083342396161</c:v>
+                  <c:v>0.174252393612335</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>0.0238916029099264</c:v>
+                  <c:v>0.174304355647055</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>0.02387542829478</c:v>
+                  <c:v>0.17435988820855</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>0.0238608246259211</c:v>
+                  <c:v>0.174419394495838</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>0.0238485753766971</c:v>
+                  <c:v>0.174483359377567</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>0.0238397561485741</c:v>
+                  <c:v>0.174552368894824</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>0.0238363134175692</c:v>
+                  <c:v>0.174627135004826</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
         <c:ser>
-          <c:idx val="6"/>
-          <c:order val="6"/>
+          <c:idx val="4"/>
+          <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$G$1</c:f>
+              <c:f>Sheet1!$E$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>6-6 RMSE</c:v>
+                  <c:v>6-5 RMSE</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2748,207 +2810,207 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$G$2:$G$62</c:f>
+              <c:f>Sheet1!$E$2:$E$62</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="61"/>
                 <c:pt idx="0">
-                  <c:v>0.569168139449575</c:v>
+                  <c:v>0.169241275988439</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.376685604948931</c:v>
+                  <c:v>0.156973001515738</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.371887779934286</c:v>
+                  <c:v>0.155885720566241</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.369579409428629</c:v>
+                  <c:v>0.156287576358033</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.368116874116947</c:v>
+                  <c:v>0.156539655488187</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.367077160839816</c:v>
+                  <c:v>0.156746298532659</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.366286998575045</c:v>
+                  <c:v>0.156946764427646</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.365659500279336</c:v>
+                  <c:v>0.157113986953844</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.365145211569558</c:v>
+                  <c:v>0.157234787280885</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.364713477080186</c:v>
+                  <c:v>0.157290948761065</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.364344116476411</c:v>
+                  <c:v>0.157237667018754</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.364023237238352</c:v>
+                  <c:v>0.157097477721355</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.363740933886453</c:v>
+                  <c:v>0.156950108101871</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.363489937506877</c:v>
+                  <c:v>0.156775342793769</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.363264782254078</c:v>
+                  <c:v>0.156479924462197</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.363061270288603</c:v>
+                  <c:v>0.156100854897301</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.362876117155491</c:v>
+                  <c:v>0.155728108838255</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.362706710365757</c:v>
+                  <c:v>0.155255506279528</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.362550941185391</c:v>
+                  <c:v>0.155766786902874</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.362407084998469</c:v>
+                  <c:v>0.157678785842452</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0.362273714628085</c:v>
+                  <c:v>0.15909211723042</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>0.362149636468458</c:v>
+                  <c:v>0.160431748627047</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>0.362033842692052</c:v>
+                  <c:v>0.161247059341444</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>0.36192547497298</c:v>
+                  <c:v>0.161192459601665</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>0.361823796587286</c:v>
+                  <c:v>0.159445048188595</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>0.36172817069317</c:v>
+                  <c:v>0.15803822863541</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>0.361638043230761</c:v>
+                  <c:v>0.157556503666126</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>0.361552929317659</c:v>
+                  <c:v>0.157193905253803</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>0.361472402320379</c:v>
+                  <c:v>0.156635723940393</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>0.361396084996153</c:v>
+                  <c:v>0.155984654824021</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>0.361323642252776</c:v>
+                  <c:v>0.155433243496393</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>0.361254775184879</c:v>
+                  <c:v>0.155035155721611</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>0.361189216126051</c:v>
+                  <c:v>0.154751782754102</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>0.361126724516127</c:v>
+                  <c:v>0.154542031586776</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>0.361067083427636</c:v>
+                  <c:v>0.154383330815537</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>0.361010096629157</c:v>
+                  <c:v>0.154264300036061</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>0.360955586088985</c:v>
+                  <c:v>0.154178545084271</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>0.360903389842191</c:v>
+                  <c:v>0.154125234678153</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>0.360853360159398</c:v>
+                  <c:v>0.154116126510043</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>0.36080536196749</c:v>
+                  <c:v>0.154168632120786</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>0.360759271481811</c:v>
+                  <c:v>0.154271742278836</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>0.360714975016784</c:v>
+                  <c:v>0.15439510051163</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>0.360672367947764</c:v>
+                  <c:v>0.154513454377253</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>0.360631353801669</c:v>
+                  <c:v>0.154613697166789</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>0.360591843457734</c:v>
+                  <c:v>0.154692036875237</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>0.360553754442779</c:v>
+                  <c:v>0.154749191540852</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>0.360517010307969</c:v>
+                  <c:v>0.15478727228059</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>0.360481540076009</c:v>
+                  <c:v>0.154808503033178</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>0.360447277749513</c:v>
+                  <c:v>0.154814868522846</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>0.360414161872603</c:v>
+                  <c:v>0.154808056572575</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>0.360382135139023</c:v>
+                  <c:v>0.154789468597659</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>0.360351144040986</c:v>
+                  <c:v>0.154760290373655</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>0.36032113855382</c:v>
+                  <c:v>0.154721691492993</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>0.360292071852134</c:v>
+                  <c:v>0.154675205091879</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>0.360263900053831</c:v>
+                  <c:v>0.154623200845203</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>0.360236581988775</c:v>
+                  <c:v>0.154569087821357</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>0.360210078989332</c:v>
+                  <c:v>0.15451675732677</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>0.360184354700378</c:v>
+                  <c:v>0.154469494159595</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>0.360159374906653</c:v>
+                  <c:v>0.154429839657681</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>0.360135107375603</c:v>
+                  <c:v>0.154401282859224</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>0.360111521714119</c:v>
+                  <c:v>0.154390133809026</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
         <c:ser>
-          <c:idx val="7"/>
-          <c:order val="7"/>
+          <c:idx val="6"/>
+          <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$H$1</c:f>
+              <c:f>Sheet1!$G$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>6-6 MSE</c:v>
+                  <c:v>6-6 RMSE</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -3152,217 +3214,217 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$H$2:$H$62</c:f>
+              <c:f>Sheet1!$G$2:$G$62</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="61"/>
                 <c:pt idx="0">
-                  <c:v>0.323952370964491</c:v>
+                  <c:v>0.569168139449575</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.141892044975742</c:v>
+                  <c:v>0.376685604948931</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.138300520864452</c:v>
+                  <c:v>0.371887779934286</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.136588939873614</c:v>
+                  <c:v>0.369579409428629</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.135510033009632</c:v>
+                  <c:v>0.368116874116947</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.13474564201022</c:v>
+                  <c:v>0.367077160839816</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.134166165325115</c:v>
+                  <c:v>0.366286998575045</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.133706870144534</c:v>
+                  <c:v>0.365659500279336</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.133331025532177</c:v>
+                  <c:v>0.365145211569558</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.133015920363919</c:v>
+                  <c:v>0.364713477080186</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.132746635210976</c:v>
+                  <c:v>0.364344116476411</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.132512917249489</c:v>
+                  <c:v>0.364023237238352</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.132307466984589</c:v>
+                  <c:v>0.363740933886453</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.132124934668753</c:v>
+                  <c:v>0.363489937506877</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.131961302026102</c:v>
+                  <c:v>0.363264782254078</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.131813485983574</c:v>
+                  <c:v>0.363061270288603</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.131679076401845</c:v>
+                  <c:v>0.362876117155491</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.131556157744349</c:v>
+                  <c:v>0.362706710365757</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.131443184954413</c:v>
+                  <c:v>0.362550941185391</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.131338895257088</c:v>
+                  <c:v>0.362407084998469</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0.131242244310431</c:v>
+                  <c:v>0.362273714628085</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>0.131152359194236</c:v>
+                  <c:v>0.362149636468458</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>0.131068503254373</c:v>
+                  <c:v>0.362033842692052</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>0.130990049434417</c:v>
+                  <c:v>0.36192547497298</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>0.130916459776837</c:v>
+                  <c:v>0.361823796587286</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>0.130847269473027</c:v>
+                  <c:v>0.36172817069317</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>0.130782074311773</c:v>
+                  <c:v>0.361638043230761</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>0.13072052069818</c:v>
+                  <c:v>0.361552929317659</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>0.130662297639266</c:v>
+                  <c:v>0.361472402320379</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>0.130607130250547</c:v>
+                  <c:v>0.361396084996153</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>0.130554774450812</c:v>
+                  <c:v>0.361323642252776</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>0.130505012593877</c:v>
+                  <c:v>0.361254775184879</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>0.130457649845751</c:v>
+                  <c:v>0.361189216126051</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>0.130412511159747</c:v>
+                  <c:v>0.361126724516127</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>0.13036943873494</c:v>
+                  <c:v>0.361067083427636</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>0.130328289868193</c:v>
+                  <c:v>0.361010096629157</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>0.130288935128842</c:v>
+                  <c:v>0.360955586088985</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>0.130251256799584</c:v>
+                  <c:v>0.360903389842191</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>0.130215147538328</c:v>
+                  <c:v>0.360853360159398</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>0.130180509224491</c:v>
+                  <c:v>0.36080536196749</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>0.130147251960087</c:v>
+                  <c:v>0.360759271481811</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>0.130115293201359</c:v>
+                  <c:v>0.360714975016784</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>0.130084557001047</c:v>
+                  <c:v>0.360672367947764</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>0.130054973344825</c:v>
+                  <c:v>0.360631353801669</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>0.130026477568246</c:v>
+                  <c:v>0.360591843457734</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>0.129999009842784</c:v>
+                  <c:v>0.360553754442779</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>0.129972514721396</c:v>
+                  <c:v>0.360517010307969</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>0.129946940735571</c:v>
+                  <c:v>0.360481540076009</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>0.129922240037034</c:v>
+                  <c:v>0.360447277749513</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>0.129898368078331</c:v>
+                  <c:v>0.360414161872603</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>0.129875283327361</c:v>
+                  <c:v>0.360382135139023</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>0.129852947011647</c:v>
+                  <c:v>0.360351144040986</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>0.129831322888721</c:v>
+                  <c:v>0.36032113855382</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>0.129810377039503</c:v>
+                  <c:v>0.360292071852134</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>0.129790077681997</c:v>
+                  <c:v>0.360263900053831</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>0.129770395002955</c:v>
+                  <c:v>0.360236581988775</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>0.129751301005501</c:v>
+                  <c:v>0.360210078989332</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>0.129732769370928</c:v>
+                  <c:v>0.360184354700378</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>0.129714775333151</c:v>
+                  <c:v>0.360159374906653</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>0.129697295564437</c:v>
+                  <c:v>0.360135107375603</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>0.129680308071258</c:v>
+                  <c:v>0.360111521714119</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="276873080"/>
-        <c:axId val="277629720"/>
+        <c:axId val="289783144"/>
+        <c:axId val="289781928"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="276873080"/>
+        <c:axId val="289783144"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="277629720"/>
+        <c:crossAx val="289781928"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="277629720"/>
+        <c:axId val="289781928"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3370,7 +3432,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="276873080"/>
+        <c:crossAx val="289783144"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="0.01"/>
@@ -3395,16 +3457,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>406400</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>127000</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>931333</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>609600</xdr:colOff>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>186266</xdr:colOff>
       <xdr:row>47</xdr:row>
-      <xdr:rowOff>60960</xdr:rowOff>
+      <xdr:rowOff>128693</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3418,6 +3480,36 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>863600</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>74507</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>118533</xdr:colOff>
+      <xdr:row>95</xdr:row>
+      <xdr:rowOff>1694</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -3746,10 +3838,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
-  <dimension ref="A1:I62"/>
+  <dimension ref="A1:O62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B21" zoomScale="125" workbookViewId="0">
-      <selection activeCell="D51" sqref="D51"/>
+    <sheetView tabSelected="1" zoomScale="75" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -5146,7 +5238,7 @@
         <v>23000</v>
       </c>
     </row>
-    <row r="49" spans="1:9">
+    <row r="49" spans="1:15">
       <c r="A49">
         <v>0.15619941605349599</v>
       </c>
@@ -5175,7 +5267,7 @@
         <v>23500</v>
       </c>
     </row>
-    <row r="50" spans="1:9">
+    <row r="50" spans="1:15">
       <c r="A50">
         <v>0.15619669203285599</v>
       </c>
@@ -5204,7 +5296,7 @@
         <v>24000</v>
       </c>
     </row>
-    <row r="51" spans="1:9">
+    <row r="51" spans="1:15">
       <c r="A51">
         <v>0.15619414077431701</v>
       </c>
@@ -5233,7 +5325,7 @@
         <v>24500</v>
       </c>
     </row>
-    <row r="52" spans="1:9">
+    <row r="52" spans="1:15">
       <c r="A52">
         <v>0.15619174217899201</v>
       </c>
@@ -5262,7 +5354,7 @@
         <v>25000</v>
       </c>
     </row>
-    <row r="53" spans="1:9">
+    <row r="53" spans="1:15">
       <c r="A53">
         <v>0.15618947953661</v>
       </c>
@@ -5291,7 +5383,7 @@
         <v>25500</v>
       </c>
     </row>
-    <row r="54" spans="1:9">
+    <row r="54" spans="1:15">
       <c r="A54">
         <v>0.15618733891075301</v>
       </c>
@@ -5320,7 +5412,7 @@
         <v>26000</v>
       </c>
     </row>
-    <row r="55" spans="1:9">
+    <row r="55" spans="1:15">
       <c r="A55">
         <v>0.156185308635994</v>
       </c>
@@ -5349,7 +5441,7 @@
         <v>26500</v>
       </c>
     </row>
-    <row r="56" spans="1:9">
+    <row r="56" spans="1:15">
       <c r="A56">
         <v>0.156183378906252</v>
       </c>
@@ -5378,7 +5470,7 @@
         <v>27000</v>
       </c>
     </row>
-    <row r="57" spans="1:9">
+    <row r="57" spans="1:15">
       <c r="A57">
         <v>0.156181541437664</v>
       </c>
@@ -5407,7 +5499,7 @@
         <v>27500</v>
       </c>
     </row>
-    <row r="58" spans="1:9">
+    <row r="58" spans="1:15">
       <c r="A58">
         <v>0.15617978919249201</v>
       </c>
@@ -5436,7 +5528,7 @@
         <v>28000</v>
       </c>
     </row>
-    <row r="59" spans="1:9">
+    <row r="59" spans="1:15">
       <c r="A59">
         <v>0.15617811615307001</v>
       </c>
@@ -5465,7 +5557,7 @@
         <v>28500</v>
       </c>
     </row>
-    <row r="60" spans="1:9">
+    <row r="60" spans="1:15">
       <c r="A60">
         <v>0.15617651713683101</v>
       </c>
@@ -5494,7 +5586,7 @@
         <v>29000</v>
       </c>
     </row>
-    <row r="61" spans="1:9">
+    <row r="61" spans="1:15">
       <c r="A61">
         <v>0.156174987645053</v>
       </c>
@@ -5522,8 +5614,11 @@
       <c r="I61">
         <v>29500</v>
       </c>
-    </row>
-    <row r="62" spans="1:9">
+      <c r="O61" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="62" spans="1:15">
       <c r="A62">
         <v>0.15617352373930701</v>
       </c>
@@ -5553,7 +5648,6 @@
       </c>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <drawing r:id="rId1"/>

</xml_diff>